<commit_message>
[210714] UPDATE 작업 스케쥴러.xlsx
</commit_message>
<xml_diff>
--- a/project/Excel/작업 스케쥴러.xlsx
+++ b/project/Excel/작업 스케쥴러.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SHOESFLY\project\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DANOMALY\SHOESFLY\project\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -253,7 +253,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -308,8 +308,15 @@
       <family val="3"/>
       <charset val="129"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="나눔고딕코딩"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -394,6 +401,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="35">
     <border>
@@ -847,7 +860,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -944,6 +957,78 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -953,24 +1038,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="13" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -980,58 +1047,22 @@
     <xf numFmtId="0" fontId="2" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1316,8 +1347,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q29" sqref="Q29"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L37" sqref="L37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.3"/>
@@ -1330,89 +1361,89 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A1" s="55"/>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="54" t="s">
+      <c r="A1" s="41"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
-      <c r="P1" s="54"/>
-      <c r="Q1" s="54"/>
-      <c r="R1" s="54"/>
-      <c r="S1" s="54"/>
-      <c r="T1" s="54"/>
-      <c r="U1" s="54"/>
-      <c r="V1" s="54"/>
-      <c r="W1" s="54"/>
-      <c r="X1" s="54"/>
-      <c r="Y1" s="54"/>
-      <c r="Z1" s="54"/>
-      <c r="AA1" s="54"/>
-      <c r="AB1" s="54" t="s">
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="37"/>
+      <c r="P1" s="37"/>
+      <c r="Q1" s="37"/>
+      <c r="R1" s="37"/>
+      <c r="S1" s="37"/>
+      <c r="T1" s="37"/>
+      <c r="U1" s="37"/>
+      <c r="V1" s="37"/>
+      <c r="W1" s="37"/>
+      <c r="X1" s="37"/>
+      <c r="Y1" s="37"/>
+      <c r="Z1" s="37"/>
+      <c r="AA1" s="37"/>
+      <c r="AB1" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="AC1" s="54"/>
-      <c r="AD1" s="54"/>
-      <c r="AE1" s="54"/>
+      <c r="AC1" s="37"/>
+      <c r="AD1" s="37"/>
+      <c r="AE1" s="37"/>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A2" s="55"/>
-      <c r="B2" s="55"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="54" t="s">
+      <c r="A2" s="41"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54" t="s">
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54" t="s">
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="54"/>
-      <c r="R2" s="54"/>
-      <c r="S2" s="54"/>
-      <c r="T2" s="54"/>
-      <c r="U2" s="54" t="s">
+      <c r="O2" s="37"/>
+      <c r="P2" s="37"/>
+      <c r="Q2" s="37"/>
+      <c r="R2" s="37"/>
+      <c r="S2" s="37"/>
+      <c r="T2" s="37"/>
+      <c r="U2" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="V2" s="54"/>
-      <c r="W2" s="54"/>
-      <c r="X2" s="54"/>
-      <c r="Y2" s="54"/>
-      <c r="Z2" s="54"/>
-      <c r="AA2" s="54"/>
-      <c r="AB2" s="54" t="s">
+      <c r="V2" s="37"/>
+      <c r="W2" s="37"/>
+      <c r="X2" s="37"/>
+      <c r="Y2" s="37"/>
+      <c r="Z2" s="37"/>
+      <c r="AA2" s="37"/>
+      <c r="AB2" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="AC2" s="54"/>
-      <c r="AD2" s="54"/>
-      <c r="AE2" s="54"/>
+      <c r="AC2" s="37"/>
+      <c r="AD2" s="37"/>
+      <c r="AE2" s="37"/>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A3" s="55"/>
-      <c r="B3" s="55"/>
-      <c r="C3" s="55"/>
+      <c r="A3" s="41"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
       <c r="D3" s="2">
         <v>8</v>
       </c>
@@ -1499,20 +1530,20 @@
       </c>
     </row>
     <row r="4" spans="1:31" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="59" t="s">
+      <c r="A4" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="61" t="s">
+      <c r="B4" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="61"/>
-      <c r="D4" s="50" t="s">
+      <c r="C4" s="33"/>
+      <c r="D4" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="51"/>
-      <c r="F4" s="51"/>
-      <c r="G4" s="51"/>
-      <c r="H4" s="52"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="44"/>
+      <c r="H4" s="45"/>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
       <c r="K4" s="9"/>
@@ -1538,9 +1569,9 @@
       <c r="AE4" s="10"/>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A5" s="59"/>
-      <c r="B5" s="61"/>
-      <c r="C5" s="61"/>
+      <c r="A5" s="40"/>
+      <c r="B5" s="33"/>
+      <c r="C5" s="33"/>
       <c r="D5" s="30"/>
       <c r="E5" s="31"/>
       <c r="F5" s="14"/>
@@ -1571,18 +1602,18 @@
       <c r="AE5" s="14"/>
     </row>
     <row r="6" spans="1:31" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="59"/>
-      <c r="B6" s="61" t="s">
+      <c r="A6" s="40"/>
+      <c r="B6" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="61"/>
+      <c r="C6" s="33"/>
       <c r="D6" s="8"/>
-      <c r="E6" s="53" t="s">
+      <c r="E6" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="51"/>
-      <c r="G6" s="51"/>
-      <c r="H6" s="52"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="45"/>
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
       <c r="K6" s="9"/>
@@ -1608,9 +1639,9 @@
       <c r="AE6" s="10"/>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A7" s="59"/>
-      <c r="B7" s="61"/>
-      <c r="C7" s="61"/>
+      <c r="A7" s="40"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="33"/>
       <c r="D7" s="12"/>
       <c r="E7" s="31"/>
       <c r="F7" s="14"/>
@@ -1641,18 +1672,18 @@
       <c r="AE7" s="14"/>
     </row>
     <row r="8" spans="1:31" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="59" t="s">
+      <c r="A8" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="61" t="s">
+      <c r="B8" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="61"/>
-      <c r="D8" s="50" t="s">
+      <c r="C8" s="33"/>
+      <c r="D8" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="E8" s="51"/>
-      <c r="F8" s="56"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="47"/>
       <c r="G8" s="8"/>
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
@@ -1680,9 +1711,9 @@
       <c r="AE8" s="10"/>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A9" s="59"/>
-      <c r="B9" s="61"/>
-      <c r="C9" s="61"/>
+      <c r="A9" s="40"/>
+      <c r="B9" s="33"/>
+      <c r="C9" s="33"/>
       <c r="D9" s="30"/>
       <c r="E9" s="31"/>
       <c r="F9" s="14"/>
@@ -1713,23 +1744,23 @@
       <c r="AE9" s="14"/>
     </row>
     <row r="10" spans="1:31" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="59"/>
-      <c r="B10" s="61" t="s">
+      <c r="A10" s="40"/>
+      <c r="B10" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="61"/>
-      <c r="D10" s="50" t="s">
+      <c r="C10" s="33"/>
+      <c r="D10" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="E10" s="51"/>
-      <c r="F10" s="56"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="47"/>
       <c r="G10" s="8"/>
-      <c r="H10" s="53" t="s">
+      <c r="H10" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="I10" s="51"/>
-      <c r="J10" s="51"/>
-      <c r="K10" s="52"/>
+      <c r="I10" s="44"/>
+      <c r="J10" s="44"/>
+      <c r="K10" s="45"/>
       <c r="L10" s="9"/>
       <c r="M10" s="10"/>
       <c r="N10" s="8"/>
@@ -1752,14 +1783,14 @@
       <c r="AE10" s="10"/>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A11" s="59"/>
-      <c r="B11" s="61"/>
-      <c r="C11" s="61"/>
+      <c r="A11" s="40"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="33"/>
       <c r="D11" s="30"/>
       <c r="E11" s="31"/>
-      <c r="F11" s="14"/>
+      <c r="F11" s="62"/>
       <c r="G11" s="12"/>
-      <c r="H11" s="13"/>
+      <c r="H11" s="63"/>
       <c r="I11" s="13"/>
       <c r="J11" s="13"/>
       <c r="K11" s="13"/>
@@ -1785,26 +1816,26 @@
       <c r="AE11" s="14"/>
     </row>
     <row r="12" spans="1:31" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="60" t="s">
+      <c r="A12" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="47" t="s">
+      <c r="B12" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="46" t="s">
+      <c r="C12" s="34" t="s">
         <v>6</v>
       </c>
       <c r="D12" s="8"/>
       <c r="E12" s="9"/>
       <c r="F12" s="10"/>
       <c r="G12" s="8"/>
-      <c r="H12" s="38" t="s">
+      <c r="H12" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="I12" s="39"/>
-      <c r="J12" s="39"/>
-      <c r="K12" s="39"/>
-      <c r="L12" s="40"/>
+      <c r="I12" s="49"/>
+      <c r="J12" s="49"/>
+      <c r="K12" s="49"/>
+      <c r="L12" s="50"/>
       <c r="M12" s="10"/>
       <c r="N12" s="8"/>
       <c r="O12" s="9"/>
@@ -1814,13 +1845,13 @@
       <c r="S12" s="9"/>
       <c r="T12" s="10"/>
       <c r="U12" s="8"/>
-      <c r="V12" s="35" t="s">
+      <c r="V12" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="W12" s="36"/>
-      <c r="X12" s="36"/>
-      <c r="Y12" s="36"/>
-      <c r="Z12" s="37"/>
+      <c r="W12" s="52"/>
+      <c r="X12" s="52"/>
+      <c r="Y12" s="52"/>
+      <c r="Z12" s="55"/>
       <c r="AA12" s="10"/>
       <c r="AB12" s="11"/>
       <c r="AC12" s="9"/>
@@ -1828,16 +1859,16 @@
       <c r="AE12" s="10"/>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A13" s="60"/>
-      <c r="B13" s="48"/>
-      <c r="C13" s="46"/>
+      <c r="A13" s="32"/>
+      <c r="B13" s="42"/>
+      <c r="C13" s="34"/>
       <c r="D13" s="12"/>
       <c r="E13" s="13"/>
       <c r="F13" s="14"/>
       <c r="G13" s="12"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
+      <c r="H13" s="66"/>
+      <c r="I13" s="66"/>
+      <c r="J13" s="66"/>
       <c r="K13" s="13"/>
       <c r="L13" s="13"/>
       <c r="M13" s="14"/>
@@ -1861,9 +1892,9 @@
       <c r="AE13" s="14"/>
     </row>
     <row r="14" spans="1:31" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="60"/>
-      <c r="B14" s="48"/>
-      <c r="C14" s="46" t="s">
+      <c r="A14" s="32"/>
+      <c r="B14" s="42"/>
+      <c r="C14" s="34" t="s">
         <v>7</v>
       </c>
       <c r="D14" s="8"/>
@@ -1872,37 +1903,37 @@
       <c r="G14" s="8"/>
       <c r="H14" s="9"/>
       <c r="I14" s="9"/>
-      <c r="J14" s="38" t="s">
+      <c r="J14" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="K14" s="39"/>
-      <c r="L14" s="39"/>
-      <c r="M14" s="39"/>
-      <c r="N14" s="39"/>
-      <c r="O14" s="39"/>
-      <c r="P14" s="39"/>
-      <c r="Q14" s="39"/>
-      <c r="R14" s="39"/>
-      <c r="S14" s="40"/>
+      <c r="K14" s="49"/>
+      <c r="L14" s="49"/>
+      <c r="M14" s="49"/>
+      <c r="N14" s="49"/>
+      <c r="O14" s="49"/>
+      <c r="P14" s="49"/>
+      <c r="Q14" s="49"/>
+      <c r="R14" s="49"/>
+      <c r="S14" s="50"/>
       <c r="T14" s="10"/>
       <c r="U14" s="8"/>
       <c r="V14" s="9"/>
-      <c r="W14" s="35" t="s">
+      <c r="W14" s="51" t="s">
         <v>45</v>
       </c>
-      <c r="X14" s="36"/>
-      <c r="Y14" s="36"/>
-      <c r="Z14" s="36"/>
-      <c r="AA14" s="36"/>
-      <c r="AB14" s="36"/>
-      <c r="AC14" s="37"/>
+      <c r="X14" s="52"/>
+      <c r="Y14" s="52"/>
+      <c r="Z14" s="52"/>
+      <c r="AA14" s="52"/>
+      <c r="AB14" s="52"/>
+      <c r="AC14" s="55"/>
       <c r="AD14" s="9"/>
       <c r="AE14" s="10"/>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A15" s="60"/>
-      <c r="B15" s="49"/>
-      <c r="C15" s="46"/>
+      <c r="A15" s="32"/>
+      <c r="B15" s="39"/>
+      <c r="C15" s="34"/>
       <c r="D15" s="12"/>
       <c r="E15" s="13"/>
       <c r="F15" s="14"/>
@@ -1933,11 +1964,11 @@
       <c r="AE15" s="14"/>
     </row>
     <row r="16" spans="1:31" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="60"/>
-      <c r="B16" s="47" t="s">
+      <c r="A16" s="32"/>
+      <c r="B16" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="47" t="s">
+      <c r="C16" s="38" t="s">
         <v>31</v>
       </c>
       <c r="D16" s="8"/>
@@ -1945,13 +1976,13 @@
       <c r="F16" s="10"/>
       <c r="G16" s="8"/>
       <c r="H16" s="9"/>
-      <c r="I16" s="38" t="s">
+      <c r="I16" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="J16" s="39"/>
-      <c r="K16" s="39"/>
-      <c r="L16" s="39"/>
-      <c r="M16" s="45"/>
+      <c r="J16" s="49"/>
+      <c r="K16" s="49"/>
+      <c r="L16" s="49"/>
+      <c r="M16" s="54"/>
       <c r="N16" s="8"/>
       <c r="O16" s="9"/>
       <c r="P16" s="9"/>
@@ -1961,29 +1992,29 @@
       <c r="T16" s="10"/>
       <c r="U16" s="8"/>
       <c r="V16" s="9"/>
-      <c r="W16" s="35" t="s">
+      <c r="W16" s="51" t="s">
         <v>45</v>
       </c>
-      <c r="X16" s="36"/>
-      <c r="Y16" s="36"/>
-      <c r="Z16" s="36"/>
-      <c r="AA16" s="36"/>
-      <c r="AB16" s="36"/>
-      <c r="AC16" s="37"/>
+      <c r="X16" s="52"/>
+      <c r="Y16" s="52"/>
+      <c r="Z16" s="52"/>
+      <c r="AA16" s="52"/>
+      <c r="AB16" s="52"/>
+      <c r="AC16" s="55"/>
       <c r="AD16" s="9"/>
       <c r="AE16" s="10"/>
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A17" s="60"/>
-      <c r="B17" s="48"/>
-      <c r="C17" s="49"/>
+      <c r="A17" s="32"/>
+      <c r="B17" s="42"/>
+      <c r="C17" s="39"/>
       <c r="D17" s="12"/>
       <c r="E17" s="13"/>
       <c r="F17" s="14"/>
       <c r="G17" s="12"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
+      <c r="H17" s="66"/>
+      <c r="I17" s="66"/>
+      <c r="J17" s="66"/>
       <c r="K17" s="13"/>
       <c r="L17" s="13"/>
       <c r="M17" s="14"/>
@@ -2007,9 +2038,9 @@
       <c r="AE17" s="14"/>
     </row>
     <row r="18" spans="1:31" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="60"/>
-      <c r="B18" s="48"/>
-      <c r="C18" s="47" t="s">
+      <c r="A18" s="32"/>
+      <c r="B18" s="42"/>
+      <c r="C18" s="38" t="s">
         <v>9</v>
       </c>
       <c r="D18" s="8"/>
@@ -2019,36 +2050,36 @@
       <c r="H18" s="9"/>
       <c r="I18" s="9"/>
       <c r="J18" s="9"/>
-      <c r="K18" s="38" t="s">
+      <c r="K18" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="L18" s="39"/>
-      <c r="M18" s="39"/>
-      <c r="N18" s="39"/>
-      <c r="O18" s="39"/>
-      <c r="P18" s="39"/>
-      <c r="Q18" s="39"/>
-      <c r="R18" s="39"/>
-      <c r="S18" s="40"/>
+      <c r="L18" s="49"/>
+      <c r="M18" s="49"/>
+      <c r="N18" s="49"/>
+      <c r="O18" s="49"/>
+      <c r="P18" s="49"/>
+      <c r="Q18" s="49"/>
+      <c r="R18" s="49"/>
+      <c r="S18" s="50"/>
       <c r="T18" s="10"/>
       <c r="U18" s="8"/>
       <c r="V18" s="9"/>
-      <c r="W18" s="35" t="s">
+      <c r="W18" s="51" t="s">
         <v>45</v>
       </c>
-      <c r="X18" s="36"/>
-      <c r="Y18" s="36"/>
-      <c r="Z18" s="36"/>
-      <c r="AA18" s="36"/>
-      <c r="AB18" s="36"/>
-      <c r="AC18" s="37"/>
+      <c r="X18" s="52"/>
+      <c r="Y18" s="52"/>
+      <c r="Z18" s="52"/>
+      <c r="AA18" s="52"/>
+      <c r="AB18" s="52"/>
+      <c r="AC18" s="55"/>
       <c r="AD18" s="9"/>
       <c r="AE18" s="10"/>
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A19" s="60"/>
-      <c r="B19" s="48"/>
-      <c r="C19" s="49"/>
+      <c r="A19" s="32"/>
+      <c r="B19" s="42"/>
+      <c r="C19" s="39"/>
       <c r="D19" s="12"/>
       <c r="E19" s="13"/>
       <c r="F19" s="14"/>
@@ -2079,9 +2110,9 @@
       <c r="AE19" s="14"/>
     </row>
     <row r="20" spans="1:31" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="60"/>
-      <c r="B20" s="48"/>
-      <c r="C20" s="47" t="s">
+      <c r="A20" s="32"/>
+      <c r="B20" s="42"/>
+      <c r="C20" s="38" t="s">
         <v>10</v>
       </c>
       <c r="D20" s="8"/>
@@ -2091,36 +2122,36 @@
       <c r="H20" s="9"/>
       <c r="I20" s="9"/>
       <c r="J20" s="9"/>
-      <c r="K20" s="38" t="s">
+      <c r="K20" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="L20" s="39"/>
-      <c r="M20" s="39"/>
-      <c r="N20" s="39"/>
-      <c r="O20" s="39"/>
-      <c r="P20" s="39"/>
-      <c r="Q20" s="39"/>
-      <c r="R20" s="39"/>
-      <c r="S20" s="40"/>
+      <c r="L20" s="49"/>
+      <c r="M20" s="49"/>
+      <c r="N20" s="49"/>
+      <c r="O20" s="49"/>
+      <c r="P20" s="49"/>
+      <c r="Q20" s="49"/>
+      <c r="R20" s="49"/>
+      <c r="S20" s="50"/>
       <c r="T20" s="10"/>
       <c r="U20" s="8"/>
       <c r="V20" s="9"/>
-      <c r="W20" s="35" t="s">
+      <c r="W20" s="51" t="s">
         <v>45</v>
       </c>
-      <c r="X20" s="36"/>
-      <c r="Y20" s="36"/>
-      <c r="Z20" s="36"/>
-      <c r="AA20" s="36"/>
-      <c r="AB20" s="36"/>
-      <c r="AC20" s="37"/>
+      <c r="X20" s="52"/>
+      <c r="Y20" s="52"/>
+      <c r="Z20" s="52"/>
+      <c r="AA20" s="52"/>
+      <c r="AB20" s="52"/>
+      <c r="AC20" s="55"/>
       <c r="AD20" s="9"/>
       <c r="AE20" s="10"/>
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A21" s="60"/>
-      <c r="B21" s="48"/>
-      <c r="C21" s="49"/>
+      <c r="A21" s="32"/>
+      <c r="B21" s="42"/>
+      <c r="C21" s="39"/>
       <c r="D21" s="12"/>
       <c r="E21" s="13"/>
       <c r="F21" s="14"/>
@@ -2151,11 +2182,11 @@
       <c r="AE21" s="14"/>
     </row>
     <row r="22" spans="1:31" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="60"/>
-      <c r="B22" s="47" t="s">
+      <c r="A22" s="32"/>
+      <c r="B22" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="46" t="s">
+      <c r="C22" s="34" t="s">
         <v>11</v>
       </c>
       <c r="D22" s="25"/>
@@ -2164,18 +2195,18 @@
       <c r="G22" s="25"/>
       <c r="H22" s="26"/>
       <c r="I22" s="26"/>
-      <c r="J22" s="41" t="s">
+      <c r="J22" s="59" t="s">
         <v>41</v>
       </c>
-      <c r="K22" s="42"/>
-      <c r="L22" s="42"/>
-      <c r="M22" s="42"/>
-      <c r="N22" s="42"/>
-      <c r="O22" s="42"/>
-      <c r="P22" s="42"/>
-      <c r="Q22" s="42"/>
-      <c r="R22" s="42"/>
-      <c r="S22" s="43"/>
+      <c r="K22" s="60"/>
+      <c r="L22" s="60"/>
+      <c r="M22" s="60"/>
+      <c r="N22" s="60"/>
+      <c r="O22" s="60"/>
+      <c r="P22" s="60"/>
+      <c r="Q22" s="60"/>
+      <c r="R22" s="60"/>
+      <c r="S22" s="61"/>
       <c r="T22" s="27"/>
       <c r="U22" s="25"/>
       <c r="V22" s="26"/>
@@ -2190,16 +2221,16 @@
       <c r="AE22" s="27"/>
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A23" s="60"/>
-      <c r="B23" s="48"/>
-      <c r="C23" s="46"/>
+      <c r="A23" s="32"/>
+      <c r="B23" s="42"/>
+      <c r="C23" s="34"/>
       <c r="D23" s="23"/>
       <c r="E23" s="21"/>
       <c r="F23" s="22"/>
       <c r="G23" s="23"/>
-      <c r="H23" s="21"/>
-      <c r="I23" s="21"/>
-      <c r="J23" s="21"/>
+      <c r="H23" s="67"/>
+      <c r="I23" s="67"/>
+      <c r="J23" s="67"/>
       <c r="K23" s="21"/>
       <c r="L23" s="21"/>
       <c r="M23" s="22"/>
@@ -2223,9 +2254,9 @@
       <c r="AE23" s="22"/>
     </row>
     <row r="24" spans="1:31" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="60"/>
-      <c r="B24" s="48"/>
-      <c r="C24" s="46" t="s">
+      <c r="A24" s="32"/>
+      <c r="B24" s="42"/>
+      <c r="C24" s="34" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="17"/>
@@ -2241,32 +2272,32 @@
       <c r="N24" s="17"/>
       <c r="O24" s="18"/>
       <c r="P24" s="18"/>
-      <c r="Q24" s="41" t="s">
+      <c r="Q24" s="59" t="s">
         <v>43</v>
       </c>
-      <c r="R24" s="42"/>
-      <c r="S24" s="42"/>
-      <c r="T24" s="42"/>
-      <c r="U24" s="42"/>
-      <c r="V24" s="42"/>
-      <c r="W24" s="42"/>
-      <c r="X24" s="43"/>
+      <c r="R24" s="60"/>
+      <c r="S24" s="60"/>
+      <c r="T24" s="60"/>
+      <c r="U24" s="60"/>
+      <c r="V24" s="60"/>
+      <c r="W24" s="60"/>
+      <c r="X24" s="61"/>
       <c r="Y24" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="Z24" s="32" t="s">
+      <c r="Z24" s="56" t="s">
         <v>47</v>
       </c>
-      <c r="AA24" s="33"/>
-      <c r="AB24" s="33"/>
-      <c r="AC24" s="34"/>
+      <c r="AA24" s="57"/>
+      <c r="AB24" s="57"/>
+      <c r="AC24" s="58"/>
       <c r="AD24" s="18"/>
       <c r="AE24" s="19"/>
     </row>
     <row r="25" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A25" s="60"/>
-      <c r="B25" s="49"/>
-      <c r="C25" s="46"/>
+      <c r="A25" s="32"/>
+      <c r="B25" s="39"/>
+      <c r="C25" s="34"/>
       <c r="D25" s="17"/>
       <c r="E25" s="18"/>
       <c r="F25" s="19"/>
@@ -2297,11 +2328,11 @@
       <c r="AE25" s="19"/>
     </row>
     <row r="26" spans="1:31" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="60"/>
-      <c r="B26" s="46" t="s">
+      <c r="A26" s="32"/>
+      <c r="B26" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="C26" s="46" t="s">
+      <c r="C26" s="34" t="s">
         <v>17</v>
       </c>
       <c r="D26" s="8"/>
@@ -2315,32 +2346,32 @@
       <c r="L26" s="9"/>
       <c r="M26" s="10"/>
       <c r="N26" s="8"/>
-      <c r="O26" s="38" t="s">
+      <c r="O26" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="P26" s="39"/>
-      <c r="Q26" s="39"/>
-      <c r="R26" s="39"/>
-      <c r="S26" s="40"/>
+      <c r="P26" s="49"/>
+      <c r="Q26" s="49"/>
+      <c r="R26" s="49"/>
+      <c r="S26" s="50"/>
       <c r="T26" s="10"/>
       <c r="U26" s="8"/>
-      <c r="V26" s="35" t="s">
+      <c r="V26" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="W26" s="36"/>
-      <c r="X26" s="36"/>
-      <c r="Y26" s="36"/>
-      <c r="Z26" s="36"/>
-      <c r="AA26" s="36"/>
-      <c r="AB26" s="36"/>
-      <c r="AC26" s="37"/>
+      <c r="W26" s="52"/>
+      <c r="X26" s="52"/>
+      <c r="Y26" s="52"/>
+      <c r="Z26" s="52"/>
+      <c r="AA26" s="52"/>
+      <c r="AB26" s="52"/>
+      <c r="AC26" s="55"/>
       <c r="AD26" s="9"/>
       <c r="AE26" s="10"/>
     </row>
     <row r="27" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A27" s="60"/>
-      <c r="B27" s="46"/>
-      <c r="C27" s="46"/>
+      <c r="A27" s="32"/>
+      <c r="B27" s="34"/>
+      <c r="C27" s="34"/>
       <c r="D27" s="12"/>
       <c r="E27" s="13"/>
       <c r="F27" s="14"/>
@@ -2371,9 +2402,9 @@
       <c r="AE27" s="14"/>
     </row>
     <row r="28" spans="1:31" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="60"/>
-      <c r="B28" s="46"/>
-      <c r="C28" s="46" t="s">
+      <c r="A28" s="32"/>
+      <c r="B28" s="34"/>
+      <c r="C28" s="34" t="s">
         <v>16</v>
       </c>
       <c r="D28" s="8"/>
@@ -2383,43 +2414,43 @@
       <c r="H28" s="9"/>
       <c r="I28" s="9"/>
       <c r="J28" s="9"/>
-      <c r="K28" s="38" t="s">
+      <c r="K28" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="L28" s="39"/>
-      <c r="M28" s="39"/>
-      <c r="N28" s="39"/>
-      <c r="O28" s="39"/>
-      <c r="P28" s="39"/>
-      <c r="Q28" s="39"/>
-      <c r="R28" s="39"/>
-      <c r="S28" s="40"/>
+      <c r="L28" s="49"/>
+      <c r="M28" s="49"/>
+      <c r="N28" s="49"/>
+      <c r="O28" s="49"/>
+      <c r="P28" s="49"/>
+      <c r="Q28" s="49"/>
+      <c r="R28" s="49"/>
+      <c r="S28" s="50"/>
       <c r="T28" s="10"/>
       <c r="U28" s="8"/>
-      <c r="V28" s="35" t="s">
+      <c r="V28" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="W28" s="36"/>
-      <c r="X28" s="36"/>
-      <c r="Y28" s="36"/>
-      <c r="Z28" s="36"/>
-      <c r="AA28" s="36"/>
-      <c r="AB28" s="36"/>
-      <c r="AC28" s="37"/>
+      <c r="W28" s="52"/>
+      <c r="X28" s="52"/>
+      <c r="Y28" s="52"/>
+      <c r="Z28" s="52"/>
+      <c r="AA28" s="52"/>
+      <c r="AB28" s="52"/>
+      <c r="AC28" s="55"/>
       <c r="AD28" s="9"/>
       <c r="AE28" s="10"/>
     </row>
     <row r="29" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A29" s="60"/>
-      <c r="B29" s="46"/>
-      <c r="C29" s="46"/>
+      <c r="A29" s="32"/>
+      <c r="B29" s="34"/>
+      <c r="C29" s="34"/>
       <c r="D29" s="12"/>
       <c r="E29" s="13"/>
       <c r="F29" s="14"/>
       <c r="G29" s="12"/>
       <c r="H29" s="13"/>
-      <c r="I29" s="13"/>
-      <c r="J29" s="13"/>
+      <c r="I29" s="66"/>
+      <c r="J29" s="66"/>
       <c r="K29" s="13"/>
       <c r="L29" s="13"/>
       <c r="M29" s="14"/>
@@ -2443,9 +2474,9 @@
       <c r="AE29" s="14"/>
     </row>
     <row r="30" spans="1:31" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="60"/>
-      <c r="B30" s="46"/>
-      <c r="C30" s="46" t="s">
+      <c r="A30" s="32"/>
+      <c r="B30" s="34"/>
+      <c r="C30" s="34" t="s">
         <v>13</v>
       </c>
       <c r="D30" s="8"/>
@@ -2455,36 +2486,36 @@
       <c r="H30" s="9"/>
       <c r="I30" s="9"/>
       <c r="J30" s="9"/>
-      <c r="K30" s="38" t="s">
+      <c r="K30" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="L30" s="39"/>
-      <c r="M30" s="39"/>
-      <c r="N30" s="39"/>
-      <c r="O30" s="39"/>
-      <c r="P30" s="39"/>
-      <c r="Q30" s="39"/>
-      <c r="R30" s="39"/>
-      <c r="S30" s="40"/>
+      <c r="L30" s="49"/>
+      <c r="M30" s="49"/>
+      <c r="N30" s="49"/>
+      <c r="O30" s="49"/>
+      <c r="P30" s="49"/>
+      <c r="Q30" s="49"/>
+      <c r="R30" s="49"/>
+      <c r="S30" s="50"/>
       <c r="T30" s="10"/>
       <c r="U30" s="8"/>
-      <c r="V30" s="35" t="s">
+      <c r="V30" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="W30" s="36"/>
-      <c r="X30" s="36"/>
-      <c r="Y30" s="36"/>
-      <c r="Z30" s="36"/>
-      <c r="AA30" s="36"/>
-      <c r="AB30" s="36"/>
-      <c r="AC30" s="37"/>
+      <c r="W30" s="52"/>
+      <c r="X30" s="52"/>
+      <c r="Y30" s="52"/>
+      <c r="Z30" s="52"/>
+      <c r="AA30" s="52"/>
+      <c r="AB30" s="52"/>
+      <c r="AC30" s="55"/>
       <c r="AD30" s="9"/>
       <c r="AE30" s="10"/>
     </row>
     <row r="31" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A31" s="60"/>
-      <c r="B31" s="46"/>
-      <c r="C31" s="46"/>
+      <c r="A31" s="32"/>
+      <c r="B31" s="34"/>
+      <c r="C31" s="34"/>
       <c r="D31" s="12"/>
       <c r="E31" s="13"/>
       <c r="F31" s="14"/>
@@ -2515,22 +2546,22 @@
       <c r="AE31" s="14"/>
     </row>
     <row r="32" spans="1:31" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="60"/>
-      <c r="B32" s="46"/>
-      <c r="C32" s="46" t="s">
+      <c r="A32" s="32"/>
+      <c r="B32" s="34"/>
+      <c r="C32" s="34" t="s">
         <v>14</v>
       </c>
       <c r="D32" s="8"/>
       <c r="E32" s="9"/>
       <c r="F32" s="10"/>
       <c r="G32" s="8"/>
-      <c r="H32" s="38" t="s">
+      <c r="H32" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="I32" s="39"/>
-      <c r="J32" s="39"/>
-      <c r="K32" s="39"/>
-      <c r="L32" s="40"/>
+      <c r="I32" s="49"/>
+      <c r="J32" s="49"/>
+      <c r="K32" s="49"/>
+      <c r="L32" s="50"/>
       <c r="M32" s="10"/>
       <c r="N32" s="8"/>
       <c r="O32" s="9"/>
@@ -2540,29 +2571,29 @@
       <c r="S32" s="9"/>
       <c r="T32" s="10"/>
       <c r="U32" s="8"/>
-      <c r="V32" s="35" t="s">
+      <c r="V32" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="W32" s="36"/>
-      <c r="X32" s="36"/>
-      <c r="Y32" s="36"/>
-      <c r="Z32" s="36"/>
-      <c r="AA32" s="36"/>
-      <c r="AB32" s="36"/>
-      <c r="AC32" s="37"/>
+      <c r="W32" s="52"/>
+      <c r="X32" s="52"/>
+      <c r="Y32" s="52"/>
+      <c r="Z32" s="52"/>
+      <c r="AA32" s="52"/>
+      <c r="AB32" s="52"/>
+      <c r="AC32" s="55"/>
       <c r="AD32" s="9"/>
       <c r="AE32" s="10"/>
     </row>
     <row r="33" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A33" s="60"/>
-      <c r="B33" s="46"/>
-      <c r="C33" s="46"/>
+      <c r="A33" s="32"/>
+      <c r="B33" s="34"/>
+      <c r="C33" s="34"/>
       <c r="D33" s="12"/>
       <c r="E33" s="13"/>
-      <c r="F33" s="14"/>
-      <c r="G33" s="12"/>
-      <c r="H33" s="13"/>
-      <c r="I33" s="13"/>
+      <c r="F33" s="64"/>
+      <c r="G33" s="65"/>
+      <c r="H33" s="66"/>
+      <c r="I33" s="66"/>
       <c r="J33" s="13"/>
       <c r="K33" s="13"/>
       <c r="L33" s="13"/>
@@ -2587,22 +2618,22 @@
       <c r="AE33" s="14"/>
     </row>
     <row r="34" spans="1:31" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="60"/>
-      <c r="B34" s="46"/>
-      <c r="C34" s="46" t="s">
+      <c r="A34" s="32"/>
+      <c r="B34" s="34"/>
+      <c r="C34" s="34" t="s">
         <v>15</v>
       </c>
       <c r="D34" s="8"/>
       <c r="E34" s="9"/>
       <c r="F34" s="10"/>
       <c r="G34" s="8"/>
-      <c r="H34" s="38" t="s">
+      <c r="H34" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="I34" s="39"/>
-      <c r="J34" s="39"/>
-      <c r="K34" s="39"/>
-      <c r="L34" s="40"/>
+      <c r="I34" s="49"/>
+      <c r="J34" s="49"/>
+      <c r="K34" s="49"/>
+      <c r="L34" s="50"/>
       <c r="M34" s="10"/>
       <c r="N34" s="8"/>
       <c r="O34" s="9"/>
@@ -2612,13 +2643,13 @@
       <c r="S34" s="9"/>
       <c r="T34" s="10"/>
       <c r="U34" s="8"/>
-      <c r="V34" s="35" t="s">
+      <c r="V34" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="W34" s="36"/>
-      <c r="X34" s="36"/>
-      <c r="Y34" s="36"/>
-      <c r="Z34" s="37"/>
+      <c r="W34" s="52"/>
+      <c r="X34" s="52"/>
+      <c r="Y34" s="52"/>
+      <c r="Z34" s="55"/>
       <c r="AA34" s="10"/>
       <c r="AB34" s="11"/>
       <c r="AC34" s="9"/>
@@ -2626,15 +2657,15 @@
       <c r="AE34" s="10"/>
     </row>
     <row r="35" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A35" s="60"/>
-      <c r="B35" s="46"/>
-      <c r="C35" s="46"/>
+      <c r="A35" s="32"/>
+      <c r="B35" s="34"/>
+      <c r="C35" s="34"/>
       <c r="D35" s="12"/>
       <c r="E35" s="13"/>
-      <c r="F35" s="14"/>
-      <c r="G35" s="12"/>
-      <c r="H35" s="13"/>
-      <c r="I35" s="13"/>
+      <c r="F35" s="64"/>
+      <c r="G35" s="65"/>
+      <c r="H35" s="66"/>
+      <c r="I35" s="66"/>
       <c r="J35" s="13"/>
       <c r="K35" s="13"/>
       <c r="L35" s="13"/>
@@ -2659,13 +2690,13 @@
       <c r="AE35" s="14"/>
     </row>
     <row r="36" spans="1:31" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="58" t="s">
+      <c r="A36" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="B36" s="57" t="s">
+      <c r="B36" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="C36" s="57"/>
+      <c r="C36" s="35"/>
       <c r="D36" s="8"/>
       <c r="E36" s="9"/>
       <c r="F36" s="10"/>
@@ -2691,16 +2722,16 @@
       <c r="Z36" s="9"/>
       <c r="AA36" s="10"/>
       <c r="AB36" s="11"/>
-      <c r="AC36" s="35" t="s">
+      <c r="AC36" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="AD36" s="36"/>
-      <c r="AE36" s="44"/>
+      <c r="AD36" s="52"/>
+      <c r="AE36" s="53"/>
     </row>
     <row r="37" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A37" s="58"/>
-      <c r="B37" s="57"/>
-      <c r="C37" s="57"/>
+      <c r="A37" s="36"/>
+      <c r="B37" s="35"/>
+      <c r="C37" s="35"/>
       <c r="D37" s="12"/>
       <c r="E37" s="13"/>
       <c r="F37" s="14"/>
@@ -2764,51 +2795,6 @@
     </row>
   </sheetData>
   <mergeCells count="62">
-    <mergeCell ref="A12:A35"/>
-    <mergeCell ref="B10:C11"/>
-    <mergeCell ref="B8:C9"/>
-    <mergeCell ref="B6:C7"/>
-    <mergeCell ref="B4:C5"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="B36:C37"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="G2:M2"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="B26:B35"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="U2:AA2"/>
-    <mergeCell ref="AB2:AE2"/>
-    <mergeCell ref="D1:AA1"/>
-    <mergeCell ref="AB1:AE1"/>
-    <mergeCell ref="A1:C3"/>
-    <mergeCell ref="N2:T2"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="B16:B21"/>
-    <mergeCell ref="D4:H4"/>
-    <mergeCell ref="E6:H6"/>
-    <mergeCell ref="B12:B15"/>
-    <mergeCell ref="H10:K10"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="H12:L12"/>
-    <mergeCell ref="AC36:AE36"/>
-    <mergeCell ref="J14:S14"/>
-    <mergeCell ref="I16:M16"/>
-    <mergeCell ref="K18:S18"/>
-    <mergeCell ref="K20:S20"/>
-    <mergeCell ref="H32:L32"/>
     <mergeCell ref="V12:Z12"/>
     <mergeCell ref="V32:AC32"/>
     <mergeCell ref="V30:AC30"/>
@@ -2825,7 +2811,52 @@
     <mergeCell ref="W18:AC18"/>
     <mergeCell ref="W20:AC20"/>
     <mergeCell ref="Q24:X24"/>
+    <mergeCell ref="AC36:AE36"/>
+    <mergeCell ref="J14:S14"/>
+    <mergeCell ref="I16:M16"/>
+    <mergeCell ref="K18:S18"/>
+    <mergeCell ref="K20:S20"/>
+    <mergeCell ref="H32:L32"/>
     <mergeCell ref="J22:S22"/>
+    <mergeCell ref="D4:H4"/>
+    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="H12:L12"/>
+    <mergeCell ref="U2:AA2"/>
+    <mergeCell ref="AB2:AE2"/>
+    <mergeCell ref="D1:AA1"/>
+    <mergeCell ref="AB1:AE1"/>
+    <mergeCell ref="A1:C3"/>
+    <mergeCell ref="N2:T2"/>
+    <mergeCell ref="B36:C37"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:M2"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="B26:B35"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="A12:A35"/>
+    <mergeCell ref="B10:C11"/>
+    <mergeCell ref="B8:C9"/>
+    <mergeCell ref="B6:C7"/>
+    <mergeCell ref="B4:C5"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="B16:B21"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[210715] UPDATE 작업 스케쥴러.xlsx
</commit_message>
<xml_diff>
--- a/project/Excel/작업 스케쥴러.xlsx
+++ b/project/Excel/작업 스케쥴러.xlsx
@@ -957,112 +957,112 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1348,7 +1348,7 @@
   <dimension ref="A1:AE43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L37" sqref="L37"/>
+      <selection activeCell="Q35" sqref="Q35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.3"/>
@@ -1361,89 +1361,89 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A1" s="41"/>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="37" t="s">
+      <c r="A1" s="61"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="37"/>
-      <c r="O1" s="37"/>
-      <c r="P1" s="37"/>
-      <c r="Q1" s="37"/>
-      <c r="R1" s="37"/>
-      <c r="S1" s="37"/>
-      <c r="T1" s="37"/>
-      <c r="U1" s="37"/>
-      <c r="V1" s="37"/>
-      <c r="W1" s="37"/>
-      <c r="X1" s="37"/>
-      <c r="Y1" s="37"/>
-      <c r="Z1" s="37"/>
-      <c r="AA1" s="37"/>
-      <c r="AB1" s="37" t="s">
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60"/>
+      <c r="J1" s="60"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="60"/>
+      <c r="M1" s="60"/>
+      <c r="N1" s="60"/>
+      <c r="O1" s="60"/>
+      <c r="P1" s="60"/>
+      <c r="Q1" s="60"/>
+      <c r="R1" s="60"/>
+      <c r="S1" s="60"/>
+      <c r="T1" s="60"/>
+      <c r="U1" s="60"/>
+      <c r="V1" s="60"/>
+      <c r="W1" s="60"/>
+      <c r="X1" s="60"/>
+      <c r="Y1" s="60"/>
+      <c r="Z1" s="60"/>
+      <c r="AA1" s="60"/>
+      <c r="AB1" s="60" t="s">
         <v>29</v>
       </c>
-      <c r="AC1" s="37"/>
-      <c r="AD1" s="37"/>
-      <c r="AE1" s="37"/>
+      <c r="AC1" s="60"/>
+      <c r="AD1" s="60"/>
+      <c r="AE1" s="60"/>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A2" s="41"/>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="37" t="s">
+      <c r="A2" s="61"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37" t="s">
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="37" t="s">
+      <c r="H2" s="60"/>
+      <c r="I2" s="60"/>
+      <c r="J2" s="60"/>
+      <c r="K2" s="60"/>
+      <c r="L2" s="60"/>
+      <c r="M2" s="60"/>
+      <c r="N2" s="60" t="s">
         <v>23</v>
       </c>
-      <c r="O2" s="37"/>
-      <c r="P2" s="37"/>
-      <c r="Q2" s="37"/>
-      <c r="R2" s="37"/>
-      <c r="S2" s="37"/>
-      <c r="T2" s="37"/>
-      <c r="U2" s="37" t="s">
+      <c r="O2" s="60"/>
+      <c r="P2" s="60"/>
+      <c r="Q2" s="60"/>
+      <c r="R2" s="60"/>
+      <c r="S2" s="60"/>
+      <c r="T2" s="60"/>
+      <c r="U2" s="60" t="s">
         <v>24</v>
       </c>
-      <c r="V2" s="37"/>
-      <c r="W2" s="37"/>
-      <c r="X2" s="37"/>
-      <c r="Y2" s="37"/>
-      <c r="Z2" s="37"/>
-      <c r="AA2" s="37"/>
-      <c r="AB2" s="37" t="s">
+      <c r="V2" s="60"/>
+      <c r="W2" s="60"/>
+      <c r="X2" s="60"/>
+      <c r="Y2" s="60"/>
+      <c r="Z2" s="60"/>
+      <c r="AA2" s="60"/>
+      <c r="AB2" s="60" t="s">
         <v>25</v>
       </c>
-      <c r="AC2" s="37"/>
-      <c r="AD2" s="37"/>
-      <c r="AE2" s="37"/>
+      <c r="AC2" s="60"/>
+      <c r="AD2" s="60"/>
+      <c r="AE2" s="60"/>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A3" s="41"/>
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
+      <c r="A3" s="61"/>
+      <c r="B3" s="61"/>
+      <c r="C3" s="61"/>
       <c r="D3" s="2">
         <v>8</v>
       </c>
@@ -1530,20 +1530,20 @@
       </c>
     </row>
     <row r="4" spans="1:31" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="33"/>
-      <c r="D4" s="43" t="s">
+      <c r="C4" s="67"/>
+      <c r="D4" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
-      <c r="G4" s="44"/>
-      <c r="H4" s="45"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="53"/>
+      <c r="H4" s="54"/>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
       <c r="K4" s="9"/>
@@ -1569,9 +1569,9 @@
       <c r="AE4" s="10"/>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A5" s="40"/>
-      <c r="B5" s="33"/>
-      <c r="C5" s="33"/>
+      <c r="A5" s="65"/>
+      <c r="B5" s="67"/>
+      <c r="C5" s="67"/>
       <c r="D5" s="30"/>
       <c r="E5" s="31"/>
       <c r="F5" s="14"/>
@@ -1602,18 +1602,18 @@
       <c r="AE5" s="14"/>
     </row>
     <row r="6" spans="1:31" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="40"/>
-      <c r="B6" s="33" t="s">
+      <c r="A6" s="65"/>
+      <c r="B6" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="33"/>
+      <c r="C6" s="67"/>
       <c r="D6" s="8"/>
-      <c r="E6" s="46" t="s">
+      <c r="E6" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="44"/>
-      <c r="G6" s="44"/>
-      <c r="H6" s="45"/>
+      <c r="F6" s="53"/>
+      <c r="G6" s="53"/>
+      <c r="H6" s="54"/>
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
       <c r="K6" s="9"/>
@@ -1639,9 +1639,9 @@
       <c r="AE6" s="10"/>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A7" s="40"/>
-      <c r="B7" s="33"/>
-      <c r="C7" s="33"/>
+      <c r="A7" s="65"/>
+      <c r="B7" s="67"/>
+      <c r="C7" s="67"/>
       <c r="D7" s="12"/>
       <c r="E7" s="31"/>
       <c r="F7" s="14"/>
@@ -1672,18 +1672,18 @@
       <c r="AE7" s="14"/>
     </row>
     <row r="8" spans="1:31" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="40" t="s">
+      <c r="A8" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="33" t="s">
+      <c r="B8" s="67" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="33"/>
-      <c r="D8" s="43" t="s">
+      <c r="C8" s="67"/>
+      <c r="D8" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="E8" s="44"/>
-      <c r="F8" s="47"/>
+      <c r="E8" s="53"/>
+      <c r="F8" s="59"/>
       <c r="G8" s="8"/>
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
@@ -1711,9 +1711,9 @@
       <c r="AE8" s="10"/>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A9" s="40"/>
-      <c r="B9" s="33"/>
-      <c r="C9" s="33"/>
+      <c r="A9" s="65"/>
+      <c r="B9" s="67"/>
+      <c r="C9" s="67"/>
       <c r="D9" s="30"/>
       <c r="E9" s="31"/>
       <c r="F9" s="14"/>
@@ -1744,23 +1744,23 @@
       <c r="AE9" s="14"/>
     </row>
     <row r="10" spans="1:31" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="40"/>
-      <c r="B10" s="33" t="s">
+      <c r="A10" s="65"/>
+      <c r="B10" s="67" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="33"/>
-      <c r="D10" s="43" t="s">
+      <c r="C10" s="67"/>
+      <c r="D10" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="E10" s="44"/>
-      <c r="F10" s="47"/>
+      <c r="E10" s="53"/>
+      <c r="F10" s="59"/>
       <c r="G10" s="8"/>
-      <c r="H10" s="46" t="s">
+      <c r="H10" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="I10" s="44"/>
-      <c r="J10" s="44"/>
-      <c r="K10" s="45"/>
+      <c r="I10" s="53"/>
+      <c r="J10" s="53"/>
+      <c r="K10" s="54"/>
       <c r="L10" s="9"/>
       <c r="M10" s="10"/>
       <c r="N10" s="8"/>
@@ -1783,14 +1783,14 @@
       <c r="AE10" s="10"/>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A11" s="40"/>
-      <c r="B11" s="33"/>
-      <c r="C11" s="33"/>
+      <c r="A11" s="65"/>
+      <c r="B11" s="67"/>
+      <c r="C11" s="67"/>
       <c r="D11" s="30"/>
       <c r="E11" s="31"/>
-      <c r="F11" s="62"/>
+      <c r="F11" s="32"/>
       <c r="G11" s="12"/>
-      <c r="H11" s="63"/>
+      <c r="H11" s="33"/>
       <c r="I11" s="13"/>
       <c r="J11" s="13"/>
       <c r="K11" s="13"/>
@@ -1816,26 +1816,26 @@
       <c r="AE11" s="14"/>
     </row>
     <row r="12" spans="1:31" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="32" t="s">
+      <c r="A12" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="38" t="s">
+      <c r="B12" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="34" t="s">
+      <c r="C12" s="64" t="s">
         <v>6</v>
       </c>
       <c r="D12" s="8"/>
       <c r="E12" s="9"/>
       <c r="F12" s="10"/>
       <c r="G12" s="8"/>
-      <c r="H12" s="48" t="s">
+      <c r="H12" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="I12" s="49"/>
-      <c r="J12" s="49"/>
-      <c r="K12" s="49"/>
-      <c r="L12" s="50"/>
+      <c r="I12" s="42"/>
+      <c r="J12" s="42"/>
+      <c r="K12" s="42"/>
+      <c r="L12" s="43"/>
       <c r="M12" s="10"/>
       <c r="N12" s="8"/>
       <c r="O12" s="9"/>
@@ -1845,13 +1845,13 @@
       <c r="S12" s="9"/>
       <c r="T12" s="10"/>
       <c r="U12" s="8"/>
-      <c r="V12" s="51" t="s">
+      <c r="V12" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="W12" s="52"/>
-      <c r="X12" s="52"/>
-      <c r="Y12" s="52"/>
-      <c r="Z12" s="55"/>
+      <c r="W12" s="39"/>
+      <c r="X12" s="39"/>
+      <c r="Y12" s="39"/>
+      <c r="Z12" s="40"/>
       <c r="AA12" s="10"/>
       <c r="AB12" s="11"/>
       <c r="AC12" s="9"/>
@@ -1859,16 +1859,16 @@
       <c r="AE12" s="10"/>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A13" s="32"/>
-      <c r="B13" s="42"/>
-      <c r="C13" s="34"/>
+      <c r="A13" s="66"/>
+      <c r="B13" s="57"/>
+      <c r="C13" s="64"/>
       <c r="D13" s="12"/>
       <c r="E13" s="13"/>
       <c r="F13" s="14"/>
       <c r="G13" s="12"/>
-      <c r="H13" s="66"/>
-      <c r="I13" s="66"/>
-      <c r="J13" s="66"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="36"/>
+      <c r="J13" s="36"/>
       <c r="K13" s="13"/>
       <c r="L13" s="13"/>
       <c r="M13" s="14"/>
@@ -1892,9 +1892,9 @@
       <c r="AE13" s="14"/>
     </row>
     <row r="14" spans="1:31" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="32"/>
-      <c r="B14" s="42"/>
-      <c r="C14" s="34" t="s">
+      <c r="A14" s="66"/>
+      <c r="B14" s="57"/>
+      <c r="C14" s="64" t="s">
         <v>7</v>
       </c>
       <c r="D14" s="8"/>
@@ -1903,44 +1903,44 @@
       <c r="G14" s="8"/>
       <c r="H14" s="9"/>
       <c r="I14" s="9"/>
-      <c r="J14" s="48" t="s">
+      <c r="J14" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="K14" s="49"/>
-      <c r="L14" s="49"/>
-      <c r="M14" s="49"/>
-      <c r="N14" s="49"/>
-      <c r="O14" s="49"/>
-      <c r="P14" s="49"/>
-      <c r="Q14" s="49"/>
-      <c r="R14" s="49"/>
-      <c r="S14" s="50"/>
+      <c r="K14" s="42"/>
+      <c r="L14" s="42"/>
+      <c r="M14" s="42"/>
+      <c r="N14" s="42"/>
+      <c r="O14" s="42"/>
+      <c r="P14" s="42"/>
+      <c r="Q14" s="42"/>
+      <c r="R14" s="42"/>
+      <c r="S14" s="43"/>
       <c r="T14" s="10"/>
       <c r="U14" s="8"/>
       <c r="V14" s="9"/>
-      <c r="W14" s="51" t="s">
+      <c r="W14" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="X14" s="52"/>
-      <c r="Y14" s="52"/>
-      <c r="Z14" s="52"/>
-      <c r="AA14" s="52"/>
-      <c r="AB14" s="52"/>
-      <c r="AC14" s="55"/>
+      <c r="X14" s="39"/>
+      <c r="Y14" s="39"/>
+      <c r="Z14" s="39"/>
+      <c r="AA14" s="39"/>
+      <c r="AB14" s="39"/>
+      <c r="AC14" s="40"/>
       <c r="AD14" s="9"/>
       <c r="AE14" s="10"/>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A15" s="32"/>
-      <c r="B15" s="39"/>
-      <c r="C15" s="34"/>
+      <c r="A15" s="66"/>
+      <c r="B15" s="58"/>
+      <c r="C15" s="64"/>
       <c r="D15" s="12"/>
       <c r="E15" s="13"/>
       <c r="F15" s="14"/>
       <c r="G15" s="12"/>
       <c r="H15" s="13"/>
       <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
+      <c r="J15" s="36"/>
       <c r="K15" s="13"/>
       <c r="L15" s="13"/>
       <c r="M15" s="14"/>
@@ -1964,11 +1964,11 @@
       <c r="AE15" s="14"/>
     </row>
     <row r="16" spans="1:31" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="32"/>
-      <c r="B16" s="38" t="s">
+      <c r="A16" s="66"/>
+      <c r="B16" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="38" t="s">
+      <c r="C16" s="56" t="s">
         <v>31</v>
       </c>
       <c r="D16" s="8"/>
@@ -1976,13 +1976,13 @@
       <c r="F16" s="10"/>
       <c r="G16" s="8"/>
       <c r="H16" s="9"/>
-      <c r="I16" s="48" t="s">
+      <c r="I16" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="J16" s="49"/>
-      <c r="K16" s="49"/>
-      <c r="L16" s="49"/>
-      <c r="M16" s="54"/>
+      <c r="J16" s="42"/>
+      <c r="K16" s="42"/>
+      <c r="L16" s="42"/>
+      <c r="M16" s="51"/>
       <c r="N16" s="8"/>
       <c r="O16" s="9"/>
       <c r="P16" s="9"/>
@@ -1992,29 +1992,29 @@
       <c r="T16" s="10"/>
       <c r="U16" s="8"/>
       <c r="V16" s="9"/>
-      <c r="W16" s="51" t="s">
+      <c r="W16" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="X16" s="52"/>
-      <c r="Y16" s="52"/>
-      <c r="Z16" s="52"/>
-      <c r="AA16" s="52"/>
-      <c r="AB16" s="52"/>
-      <c r="AC16" s="55"/>
+      <c r="X16" s="39"/>
+      <c r="Y16" s="39"/>
+      <c r="Z16" s="39"/>
+      <c r="AA16" s="39"/>
+      <c r="AB16" s="39"/>
+      <c r="AC16" s="40"/>
       <c r="AD16" s="9"/>
       <c r="AE16" s="10"/>
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A17" s="32"/>
-      <c r="B17" s="42"/>
-      <c r="C17" s="39"/>
+      <c r="A17" s="66"/>
+      <c r="B17" s="57"/>
+      <c r="C17" s="58"/>
       <c r="D17" s="12"/>
       <c r="E17" s="13"/>
       <c r="F17" s="14"/>
       <c r="G17" s="12"/>
-      <c r="H17" s="66"/>
-      <c r="I17" s="66"/>
-      <c r="J17" s="66"/>
+      <c r="H17" s="36"/>
+      <c r="I17" s="36"/>
+      <c r="J17" s="36"/>
       <c r="K17" s="13"/>
       <c r="L17" s="13"/>
       <c r="M17" s="14"/>
@@ -2038,9 +2038,9 @@
       <c r="AE17" s="14"/>
     </row>
     <row r="18" spans="1:31" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="32"/>
-      <c r="B18" s="42"/>
-      <c r="C18" s="38" t="s">
+      <c r="A18" s="66"/>
+      <c r="B18" s="57"/>
+      <c r="C18" s="56" t="s">
         <v>9</v>
       </c>
       <c r="D18" s="8"/>
@@ -2050,36 +2050,36 @@
       <c r="H18" s="9"/>
       <c r="I18" s="9"/>
       <c r="J18" s="9"/>
-      <c r="K18" s="48" t="s">
+      <c r="K18" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="L18" s="49"/>
-      <c r="M18" s="49"/>
-      <c r="N18" s="49"/>
-      <c r="O18" s="49"/>
-      <c r="P18" s="49"/>
-      <c r="Q18" s="49"/>
-      <c r="R18" s="49"/>
-      <c r="S18" s="50"/>
+      <c r="L18" s="42"/>
+      <c r="M18" s="42"/>
+      <c r="N18" s="42"/>
+      <c r="O18" s="42"/>
+      <c r="P18" s="42"/>
+      <c r="Q18" s="42"/>
+      <c r="R18" s="42"/>
+      <c r="S18" s="43"/>
       <c r="T18" s="10"/>
       <c r="U18" s="8"/>
       <c r="V18" s="9"/>
-      <c r="W18" s="51" t="s">
+      <c r="W18" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="X18" s="52"/>
-      <c r="Y18" s="52"/>
-      <c r="Z18" s="52"/>
-      <c r="AA18" s="52"/>
-      <c r="AB18" s="52"/>
-      <c r="AC18" s="55"/>
+      <c r="X18" s="39"/>
+      <c r="Y18" s="39"/>
+      <c r="Z18" s="39"/>
+      <c r="AA18" s="39"/>
+      <c r="AB18" s="39"/>
+      <c r="AC18" s="40"/>
       <c r="AD18" s="9"/>
       <c r="AE18" s="10"/>
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A19" s="32"/>
-      <c r="B19" s="42"/>
-      <c r="C19" s="39"/>
+      <c r="A19" s="66"/>
+      <c r="B19" s="57"/>
+      <c r="C19" s="58"/>
       <c r="D19" s="12"/>
       <c r="E19" s="13"/>
       <c r="F19" s="14"/>
@@ -2110,9 +2110,9 @@
       <c r="AE19" s="14"/>
     </row>
     <row r="20" spans="1:31" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="32"/>
-      <c r="B20" s="42"/>
-      <c r="C20" s="38" t="s">
+      <c r="A20" s="66"/>
+      <c r="B20" s="57"/>
+      <c r="C20" s="56" t="s">
         <v>10</v>
       </c>
       <c r="D20" s="8"/>
@@ -2122,36 +2122,36 @@
       <c r="H20" s="9"/>
       <c r="I20" s="9"/>
       <c r="J20" s="9"/>
-      <c r="K20" s="48" t="s">
+      <c r="K20" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="L20" s="49"/>
-      <c r="M20" s="49"/>
-      <c r="N20" s="49"/>
-      <c r="O20" s="49"/>
-      <c r="P20" s="49"/>
-      <c r="Q20" s="49"/>
-      <c r="R20" s="49"/>
-      <c r="S20" s="50"/>
+      <c r="L20" s="42"/>
+      <c r="M20" s="42"/>
+      <c r="N20" s="42"/>
+      <c r="O20" s="42"/>
+      <c r="P20" s="42"/>
+      <c r="Q20" s="42"/>
+      <c r="R20" s="42"/>
+      <c r="S20" s="43"/>
       <c r="T20" s="10"/>
       <c r="U20" s="8"/>
       <c r="V20" s="9"/>
-      <c r="W20" s="51" t="s">
+      <c r="W20" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="X20" s="52"/>
-      <c r="Y20" s="52"/>
-      <c r="Z20" s="52"/>
-      <c r="AA20" s="52"/>
-      <c r="AB20" s="52"/>
-      <c r="AC20" s="55"/>
+      <c r="X20" s="39"/>
+      <c r="Y20" s="39"/>
+      <c r="Z20" s="39"/>
+      <c r="AA20" s="39"/>
+      <c r="AB20" s="39"/>
+      <c r="AC20" s="40"/>
       <c r="AD20" s="9"/>
       <c r="AE20" s="10"/>
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A21" s="32"/>
-      <c r="B21" s="42"/>
-      <c r="C21" s="39"/>
+      <c r="A21" s="66"/>
+      <c r="B21" s="57"/>
+      <c r="C21" s="58"/>
       <c r="D21" s="12"/>
       <c r="E21" s="13"/>
       <c r="F21" s="14"/>
@@ -2182,11 +2182,11 @@
       <c r="AE21" s="14"/>
     </row>
     <row r="22" spans="1:31" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="32"/>
-      <c r="B22" s="38" t="s">
+      <c r="A22" s="66"/>
+      <c r="B22" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="34" t="s">
+      <c r="C22" s="64" t="s">
         <v>11</v>
       </c>
       <c r="D22" s="25"/>
@@ -2195,18 +2195,18 @@
       <c r="G22" s="25"/>
       <c r="H22" s="26"/>
       <c r="I22" s="26"/>
-      <c r="J22" s="59" t="s">
+      <c r="J22" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="K22" s="60"/>
-      <c r="L22" s="60"/>
-      <c r="M22" s="60"/>
-      <c r="N22" s="60"/>
-      <c r="O22" s="60"/>
-      <c r="P22" s="60"/>
-      <c r="Q22" s="60"/>
-      <c r="R22" s="60"/>
-      <c r="S22" s="61"/>
+      <c r="K22" s="48"/>
+      <c r="L22" s="48"/>
+      <c r="M22" s="48"/>
+      <c r="N22" s="48"/>
+      <c r="O22" s="48"/>
+      <c r="P22" s="48"/>
+      <c r="Q22" s="48"/>
+      <c r="R22" s="48"/>
+      <c r="S22" s="49"/>
       <c r="T22" s="27"/>
       <c r="U22" s="25"/>
       <c r="V22" s="26"/>
@@ -2221,16 +2221,16 @@
       <c r="AE22" s="27"/>
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A23" s="32"/>
-      <c r="B23" s="42"/>
-      <c r="C23" s="34"/>
+      <c r="A23" s="66"/>
+      <c r="B23" s="57"/>
+      <c r="C23" s="64"/>
       <c r="D23" s="23"/>
       <c r="E23" s="21"/>
       <c r="F23" s="22"/>
       <c r="G23" s="23"/>
-      <c r="H23" s="67"/>
-      <c r="I23" s="67"/>
-      <c r="J23" s="67"/>
+      <c r="H23" s="37"/>
+      <c r="I23" s="37"/>
+      <c r="J23" s="37"/>
       <c r="K23" s="21"/>
       <c r="L23" s="21"/>
       <c r="M23" s="22"/>
@@ -2254,9 +2254,9 @@
       <c r="AE23" s="22"/>
     </row>
     <row r="24" spans="1:31" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="32"/>
-      <c r="B24" s="42"/>
-      <c r="C24" s="34" t="s">
+      <c r="A24" s="66"/>
+      <c r="B24" s="57"/>
+      <c r="C24" s="64" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="17"/>
@@ -2272,32 +2272,32 @@
       <c r="N24" s="17"/>
       <c r="O24" s="18"/>
       <c r="P24" s="18"/>
-      <c r="Q24" s="59" t="s">
+      <c r="Q24" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="R24" s="60"/>
-      <c r="S24" s="60"/>
-      <c r="T24" s="60"/>
-      <c r="U24" s="60"/>
-      <c r="V24" s="60"/>
-      <c r="W24" s="60"/>
-      <c r="X24" s="61"/>
+      <c r="R24" s="48"/>
+      <c r="S24" s="48"/>
+      <c r="T24" s="48"/>
+      <c r="U24" s="48"/>
+      <c r="V24" s="48"/>
+      <c r="W24" s="48"/>
+      <c r="X24" s="49"/>
       <c r="Y24" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="Z24" s="56" t="s">
+      <c r="Z24" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="AA24" s="57"/>
-      <c r="AB24" s="57"/>
-      <c r="AC24" s="58"/>
+      <c r="AA24" s="45"/>
+      <c r="AB24" s="45"/>
+      <c r="AC24" s="46"/>
       <c r="AD24" s="18"/>
       <c r="AE24" s="19"/>
     </row>
     <row r="25" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A25" s="32"/>
-      <c r="B25" s="39"/>
-      <c r="C25" s="34"/>
+      <c r="A25" s="66"/>
+      <c r="B25" s="58"/>
+      <c r="C25" s="64"/>
       <c r="D25" s="17"/>
       <c r="E25" s="18"/>
       <c r="F25" s="19"/>
@@ -2328,11 +2328,11 @@
       <c r="AE25" s="19"/>
     </row>
     <row r="26" spans="1:31" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="32"/>
-      <c r="B26" s="34" t="s">
+      <c r="A26" s="66"/>
+      <c r="B26" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="C26" s="34" t="s">
+      <c r="C26" s="64" t="s">
         <v>17</v>
       </c>
       <c r="D26" s="8"/>
@@ -2346,32 +2346,32 @@
       <c r="L26" s="9"/>
       <c r="M26" s="10"/>
       <c r="N26" s="8"/>
-      <c r="O26" s="48" t="s">
+      <c r="O26" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="P26" s="49"/>
-      <c r="Q26" s="49"/>
-      <c r="R26" s="49"/>
-      <c r="S26" s="50"/>
+      <c r="P26" s="42"/>
+      <c r="Q26" s="42"/>
+      <c r="R26" s="42"/>
+      <c r="S26" s="43"/>
       <c r="T26" s="10"/>
       <c r="U26" s="8"/>
-      <c r="V26" s="51" t="s">
+      <c r="V26" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="W26" s="52"/>
-      <c r="X26" s="52"/>
-      <c r="Y26" s="52"/>
-      <c r="Z26" s="52"/>
-      <c r="AA26" s="52"/>
-      <c r="AB26" s="52"/>
-      <c r="AC26" s="55"/>
+      <c r="W26" s="39"/>
+      <c r="X26" s="39"/>
+      <c r="Y26" s="39"/>
+      <c r="Z26" s="39"/>
+      <c r="AA26" s="39"/>
+      <c r="AB26" s="39"/>
+      <c r="AC26" s="40"/>
       <c r="AD26" s="9"/>
       <c r="AE26" s="10"/>
     </row>
     <row r="27" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A27" s="32"/>
-      <c r="B27" s="34"/>
-      <c r="C27" s="34"/>
+      <c r="A27" s="66"/>
+      <c r="B27" s="64"/>
+      <c r="C27" s="64"/>
       <c r="D27" s="12"/>
       <c r="E27" s="13"/>
       <c r="F27" s="14"/>
@@ -2402,9 +2402,9 @@
       <c r="AE27" s="14"/>
     </row>
     <row r="28" spans="1:31" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="32"/>
-      <c r="B28" s="34"/>
-      <c r="C28" s="34" t="s">
+      <c r="A28" s="66"/>
+      <c r="B28" s="64"/>
+      <c r="C28" s="64" t="s">
         <v>16</v>
       </c>
       <c r="D28" s="8"/>
@@ -2414,43 +2414,43 @@
       <c r="H28" s="9"/>
       <c r="I28" s="9"/>
       <c r="J28" s="9"/>
-      <c r="K28" s="48" t="s">
+      <c r="K28" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="L28" s="49"/>
-      <c r="M28" s="49"/>
-      <c r="N28" s="49"/>
-      <c r="O28" s="49"/>
-      <c r="P28" s="49"/>
-      <c r="Q28" s="49"/>
-      <c r="R28" s="49"/>
-      <c r="S28" s="50"/>
+      <c r="L28" s="42"/>
+      <c r="M28" s="42"/>
+      <c r="N28" s="42"/>
+      <c r="O28" s="42"/>
+      <c r="P28" s="42"/>
+      <c r="Q28" s="42"/>
+      <c r="R28" s="42"/>
+      <c r="S28" s="43"/>
       <c r="T28" s="10"/>
       <c r="U28" s="8"/>
-      <c r="V28" s="51" t="s">
+      <c r="V28" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="W28" s="52"/>
-      <c r="X28" s="52"/>
-      <c r="Y28" s="52"/>
-      <c r="Z28" s="52"/>
-      <c r="AA28" s="52"/>
-      <c r="AB28" s="52"/>
-      <c r="AC28" s="55"/>
+      <c r="W28" s="39"/>
+      <c r="X28" s="39"/>
+      <c r="Y28" s="39"/>
+      <c r="Z28" s="39"/>
+      <c r="AA28" s="39"/>
+      <c r="AB28" s="39"/>
+      <c r="AC28" s="40"/>
       <c r="AD28" s="9"/>
       <c r="AE28" s="10"/>
     </row>
     <row r="29" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A29" s="32"/>
-      <c r="B29" s="34"/>
-      <c r="C29" s="34"/>
+      <c r="A29" s="66"/>
+      <c r="B29" s="64"/>
+      <c r="C29" s="64"/>
       <c r="D29" s="12"/>
       <c r="E29" s="13"/>
       <c r="F29" s="14"/>
       <c r="G29" s="12"/>
       <c r="H29" s="13"/>
-      <c r="I29" s="66"/>
-      <c r="J29" s="66"/>
+      <c r="I29" s="36"/>
+      <c r="J29" s="36"/>
       <c r="K29" s="13"/>
       <c r="L29" s="13"/>
       <c r="M29" s="14"/>
@@ -2474,9 +2474,9 @@
       <c r="AE29" s="14"/>
     </row>
     <row r="30" spans="1:31" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="32"/>
-      <c r="B30" s="34"/>
-      <c r="C30" s="34" t="s">
+      <c r="A30" s="66"/>
+      <c r="B30" s="64"/>
+      <c r="C30" s="64" t="s">
         <v>13</v>
       </c>
       <c r="D30" s="8"/>
@@ -2486,36 +2486,36 @@
       <c r="H30" s="9"/>
       <c r="I30" s="9"/>
       <c r="J30" s="9"/>
-      <c r="K30" s="48" t="s">
+      <c r="K30" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="L30" s="49"/>
-      <c r="M30" s="49"/>
-      <c r="N30" s="49"/>
-      <c r="O30" s="49"/>
-      <c r="P30" s="49"/>
-      <c r="Q30" s="49"/>
-      <c r="R30" s="49"/>
-      <c r="S30" s="50"/>
+      <c r="L30" s="42"/>
+      <c r="M30" s="42"/>
+      <c r="N30" s="42"/>
+      <c r="O30" s="42"/>
+      <c r="P30" s="42"/>
+      <c r="Q30" s="42"/>
+      <c r="R30" s="42"/>
+      <c r="S30" s="43"/>
       <c r="T30" s="10"/>
       <c r="U30" s="8"/>
-      <c r="V30" s="51" t="s">
+      <c r="V30" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="W30" s="52"/>
-      <c r="X30" s="52"/>
-      <c r="Y30" s="52"/>
-      <c r="Z30" s="52"/>
-      <c r="AA30" s="52"/>
-      <c r="AB30" s="52"/>
-      <c r="AC30" s="55"/>
+      <c r="W30" s="39"/>
+      <c r="X30" s="39"/>
+      <c r="Y30" s="39"/>
+      <c r="Z30" s="39"/>
+      <c r="AA30" s="39"/>
+      <c r="AB30" s="39"/>
+      <c r="AC30" s="40"/>
       <c r="AD30" s="9"/>
       <c r="AE30" s="10"/>
     </row>
     <row r="31" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A31" s="32"/>
-      <c r="B31" s="34"/>
-      <c r="C31" s="34"/>
+      <c r="A31" s="66"/>
+      <c r="B31" s="64"/>
+      <c r="C31" s="64"/>
       <c r="D31" s="12"/>
       <c r="E31" s="13"/>
       <c r="F31" s="14"/>
@@ -2546,22 +2546,22 @@
       <c r="AE31" s="14"/>
     </row>
     <row r="32" spans="1:31" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="32"/>
-      <c r="B32" s="34"/>
-      <c r="C32" s="34" t="s">
+      <c r="A32" s="66"/>
+      <c r="B32" s="64"/>
+      <c r="C32" s="64" t="s">
         <v>14</v>
       </c>
       <c r="D32" s="8"/>
       <c r="E32" s="9"/>
       <c r="F32" s="10"/>
       <c r="G32" s="8"/>
-      <c r="H32" s="48" t="s">
+      <c r="H32" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="I32" s="49"/>
-      <c r="J32" s="49"/>
-      <c r="K32" s="49"/>
-      <c r="L32" s="50"/>
+      <c r="I32" s="42"/>
+      <c r="J32" s="42"/>
+      <c r="K32" s="42"/>
+      <c r="L32" s="43"/>
       <c r="M32" s="10"/>
       <c r="N32" s="8"/>
       <c r="O32" s="9"/>
@@ -2571,29 +2571,29 @@
       <c r="S32" s="9"/>
       <c r="T32" s="10"/>
       <c r="U32" s="8"/>
-      <c r="V32" s="51" t="s">
+      <c r="V32" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="W32" s="52"/>
-      <c r="X32" s="52"/>
-      <c r="Y32" s="52"/>
-      <c r="Z32" s="52"/>
-      <c r="AA32" s="52"/>
-      <c r="AB32" s="52"/>
-      <c r="AC32" s="55"/>
+      <c r="W32" s="39"/>
+      <c r="X32" s="39"/>
+      <c r="Y32" s="39"/>
+      <c r="Z32" s="39"/>
+      <c r="AA32" s="39"/>
+      <c r="AB32" s="39"/>
+      <c r="AC32" s="40"/>
       <c r="AD32" s="9"/>
       <c r="AE32" s="10"/>
     </row>
     <row r="33" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A33" s="32"/>
-      <c r="B33" s="34"/>
-      <c r="C33" s="34"/>
+      <c r="A33" s="66"/>
+      <c r="B33" s="64"/>
+      <c r="C33" s="64"/>
       <c r="D33" s="12"/>
       <c r="E33" s="13"/>
-      <c r="F33" s="64"/>
-      <c r="G33" s="65"/>
-      <c r="H33" s="66"/>
-      <c r="I33" s="66"/>
+      <c r="F33" s="34"/>
+      <c r="G33" s="35"/>
+      <c r="H33" s="36"/>
+      <c r="I33" s="36"/>
       <c r="J33" s="13"/>
       <c r="K33" s="13"/>
       <c r="L33" s="13"/>
@@ -2618,22 +2618,22 @@
       <c r="AE33" s="14"/>
     </row>
     <row r="34" spans="1:31" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="32"/>
-      <c r="B34" s="34"/>
-      <c r="C34" s="34" t="s">
+      <c r="A34" s="66"/>
+      <c r="B34" s="64"/>
+      <c r="C34" s="64" t="s">
         <v>15</v>
       </c>
       <c r="D34" s="8"/>
       <c r="E34" s="9"/>
       <c r="F34" s="10"/>
       <c r="G34" s="8"/>
-      <c r="H34" s="48" t="s">
+      <c r="H34" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="I34" s="49"/>
-      <c r="J34" s="49"/>
-      <c r="K34" s="49"/>
-      <c r="L34" s="50"/>
+      <c r="I34" s="42"/>
+      <c r="J34" s="42"/>
+      <c r="K34" s="42"/>
+      <c r="L34" s="43"/>
       <c r="M34" s="10"/>
       <c r="N34" s="8"/>
       <c r="O34" s="9"/>
@@ -2643,13 +2643,13 @@
       <c r="S34" s="9"/>
       <c r="T34" s="10"/>
       <c r="U34" s="8"/>
-      <c r="V34" s="51" t="s">
+      <c r="V34" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="W34" s="52"/>
-      <c r="X34" s="52"/>
-      <c r="Y34" s="52"/>
-      <c r="Z34" s="55"/>
+      <c r="W34" s="39"/>
+      <c r="X34" s="39"/>
+      <c r="Y34" s="39"/>
+      <c r="Z34" s="40"/>
       <c r="AA34" s="10"/>
       <c r="AB34" s="11"/>
       <c r="AC34" s="9"/>
@@ -2657,15 +2657,15 @@
       <c r="AE34" s="10"/>
     </row>
     <row r="35" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A35" s="32"/>
-      <c r="B35" s="34"/>
-      <c r="C35" s="34"/>
+      <c r="A35" s="66"/>
+      <c r="B35" s="64"/>
+      <c r="C35" s="64"/>
       <c r="D35" s="12"/>
       <c r="E35" s="13"/>
-      <c r="F35" s="64"/>
-      <c r="G35" s="65"/>
-      <c r="H35" s="66"/>
-      <c r="I35" s="66"/>
+      <c r="F35" s="34"/>
+      <c r="G35" s="35"/>
+      <c r="H35" s="36"/>
+      <c r="I35" s="36"/>
       <c r="J35" s="13"/>
       <c r="K35" s="13"/>
       <c r="L35" s="13"/>
@@ -2690,13 +2690,13 @@
       <c r="AE35" s="14"/>
     </row>
     <row r="36" spans="1:31" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="36" t="s">
+      <c r="A36" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="B36" s="35" t="s">
+      <c r="B36" s="62" t="s">
         <v>28</v>
       </c>
-      <c r="C36" s="35"/>
+      <c r="C36" s="62"/>
       <c r="D36" s="8"/>
       <c r="E36" s="9"/>
       <c r="F36" s="10"/>
@@ -2722,16 +2722,16 @@
       <c r="Z36" s="9"/>
       <c r="AA36" s="10"/>
       <c r="AB36" s="11"/>
-      <c r="AC36" s="51" t="s">
+      <c r="AC36" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="AD36" s="52"/>
-      <c r="AE36" s="53"/>
+      <c r="AD36" s="39"/>
+      <c r="AE36" s="50"/>
     </row>
     <row r="37" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A37" s="36"/>
-      <c r="B37" s="35"/>
-      <c r="C37" s="35"/>
+      <c r="A37" s="63"/>
+      <c r="B37" s="62"/>
+      <c r="C37" s="62"/>
       <c r="D37" s="12"/>
       <c r="E37" s="13"/>
       <c r="F37" s="14"/>
@@ -2795,6 +2795,52 @@
     </row>
   </sheetData>
   <mergeCells count="62">
+    <mergeCell ref="A12:A35"/>
+    <mergeCell ref="B10:C11"/>
+    <mergeCell ref="B8:C9"/>
+    <mergeCell ref="B6:C7"/>
+    <mergeCell ref="B4:C5"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="B16:B21"/>
+    <mergeCell ref="B36:C37"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:M2"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="B26:B35"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="U2:AA2"/>
+    <mergeCell ref="AB2:AE2"/>
+    <mergeCell ref="D1:AA1"/>
+    <mergeCell ref="AB1:AE1"/>
+    <mergeCell ref="A1:C3"/>
+    <mergeCell ref="N2:T2"/>
+    <mergeCell ref="D4:H4"/>
+    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="H12:L12"/>
+    <mergeCell ref="AC36:AE36"/>
+    <mergeCell ref="J14:S14"/>
+    <mergeCell ref="I16:M16"/>
+    <mergeCell ref="K18:S18"/>
+    <mergeCell ref="K20:S20"/>
+    <mergeCell ref="H32:L32"/>
+    <mergeCell ref="J22:S22"/>
     <mergeCell ref="V12:Z12"/>
     <mergeCell ref="V32:AC32"/>
     <mergeCell ref="V30:AC30"/>
@@ -2811,52 +2857,6 @@
     <mergeCell ref="W18:AC18"/>
     <mergeCell ref="W20:AC20"/>
     <mergeCell ref="Q24:X24"/>
-    <mergeCell ref="AC36:AE36"/>
-    <mergeCell ref="J14:S14"/>
-    <mergeCell ref="I16:M16"/>
-    <mergeCell ref="K18:S18"/>
-    <mergeCell ref="K20:S20"/>
-    <mergeCell ref="H32:L32"/>
-    <mergeCell ref="J22:S22"/>
-    <mergeCell ref="D4:H4"/>
-    <mergeCell ref="E6:H6"/>
-    <mergeCell ref="B12:B15"/>
-    <mergeCell ref="H10:K10"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="H12:L12"/>
-    <mergeCell ref="U2:AA2"/>
-    <mergeCell ref="AB2:AE2"/>
-    <mergeCell ref="D1:AA1"/>
-    <mergeCell ref="AB1:AE1"/>
-    <mergeCell ref="A1:C3"/>
-    <mergeCell ref="N2:T2"/>
-    <mergeCell ref="B36:C37"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="G2:M2"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="B26:B35"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="A12:A35"/>
-    <mergeCell ref="B10:C11"/>
-    <mergeCell ref="B8:C9"/>
-    <mergeCell ref="B6:C7"/>
-    <mergeCell ref="B4:C5"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="B16:B21"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[210716] 임시 marge를 위한 커밋
</commit_message>
<xml_diff>
--- a/project/Excel/작업 스케쥴러.xlsx
+++ b/project/Excel/작업 스케쥴러.xlsx
@@ -957,112 +957,112 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1348,7 +1348,7 @@
   <dimension ref="A1:AE43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L37" sqref="L37"/>
+      <selection activeCell="Q35" sqref="Q35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.3"/>
@@ -1361,89 +1361,89 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A1" s="41"/>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="37" t="s">
+      <c r="A1" s="61"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="37"/>
-      <c r="O1" s="37"/>
-      <c r="P1" s="37"/>
-      <c r="Q1" s="37"/>
-      <c r="R1" s="37"/>
-      <c r="S1" s="37"/>
-      <c r="T1" s="37"/>
-      <c r="U1" s="37"/>
-      <c r="V1" s="37"/>
-      <c r="W1" s="37"/>
-      <c r="X1" s="37"/>
-      <c r="Y1" s="37"/>
-      <c r="Z1" s="37"/>
-      <c r="AA1" s="37"/>
-      <c r="AB1" s="37" t="s">
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60"/>
+      <c r="J1" s="60"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="60"/>
+      <c r="M1" s="60"/>
+      <c r="N1" s="60"/>
+      <c r="O1" s="60"/>
+      <c r="P1" s="60"/>
+      <c r="Q1" s="60"/>
+      <c r="R1" s="60"/>
+      <c r="S1" s="60"/>
+      <c r="T1" s="60"/>
+      <c r="U1" s="60"/>
+      <c r="V1" s="60"/>
+      <c r="W1" s="60"/>
+      <c r="X1" s="60"/>
+      <c r="Y1" s="60"/>
+      <c r="Z1" s="60"/>
+      <c r="AA1" s="60"/>
+      <c r="AB1" s="60" t="s">
         <v>29</v>
       </c>
-      <c r="AC1" s="37"/>
-      <c r="AD1" s="37"/>
-      <c r="AE1" s="37"/>
+      <c r="AC1" s="60"/>
+      <c r="AD1" s="60"/>
+      <c r="AE1" s="60"/>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A2" s="41"/>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="37" t="s">
+      <c r="A2" s="61"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37" t="s">
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="37" t="s">
+      <c r="H2" s="60"/>
+      <c r="I2" s="60"/>
+      <c r="J2" s="60"/>
+      <c r="K2" s="60"/>
+      <c r="L2" s="60"/>
+      <c r="M2" s="60"/>
+      <c r="N2" s="60" t="s">
         <v>23</v>
       </c>
-      <c r="O2" s="37"/>
-      <c r="P2" s="37"/>
-      <c r="Q2" s="37"/>
-      <c r="R2" s="37"/>
-      <c r="S2" s="37"/>
-      <c r="T2" s="37"/>
-      <c r="U2" s="37" t="s">
+      <c r="O2" s="60"/>
+      <c r="P2" s="60"/>
+      <c r="Q2" s="60"/>
+      <c r="R2" s="60"/>
+      <c r="S2" s="60"/>
+      <c r="T2" s="60"/>
+      <c r="U2" s="60" t="s">
         <v>24</v>
       </c>
-      <c r="V2" s="37"/>
-      <c r="W2" s="37"/>
-      <c r="X2" s="37"/>
-      <c r="Y2" s="37"/>
-      <c r="Z2" s="37"/>
-      <c r="AA2" s="37"/>
-      <c r="AB2" s="37" t="s">
+      <c r="V2" s="60"/>
+      <c r="W2" s="60"/>
+      <c r="X2" s="60"/>
+      <c r="Y2" s="60"/>
+      <c r="Z2" s="60"/>
+      <c r="AA2" s="60"/>
+      <c r="AB2" s="60" t="s">
         <v>25</v>
       </c>
-      <c r="AC2" s="37"/>
-      <c r="AD2" s="37"/>
-      <c r="AE2" s="37"/>
+      <c r="AC2" s="60"/>
+      <c r="AD2" s="60"/>
+      <c r="AE2" s="60"/>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A3" s="41"/>
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
+      <c r="A3" s="61"/>
+      <c r="B3" s="61"/>
+      <c r="C3" s="61"/>
       <c r="D3" s="2">
         <v>8</v>
       </c>
@@ -1530,20 +1530,20 @@
       </c>
     </row>
     <row r="4" spans="1:31" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="33"/>
-      <c r="D4" s="43" t="s">
+      <c r="C4" s="67"/>
+      <c r="D4" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
-      <c r="G4" s="44"/>
-      <c r="H4" s="45"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="53"/>
+      <c r="H4" s="54"/>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
       <c r="K4" s="9"/>
@@ -1569,9 +1569,9 @@
       <c r="AE4" s="10"/>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A5" s="40"/>
-      <c r="B5" s="33"/>
-      <c r="C5" s="33"/>
+      <c r="A5" s="65"/>
+      <c r="B5" s="67"/>
+      <c r="C5" s="67"/>
       <c r="D5" s="30"/>
       <c r="E5" s="31"/>
       <c r="F5" s="14"/>
@@ -1602,18 +1602,18 @@
       <c r="AE5" s="14"/>
     </row>
     <row r="6" spans="1:31" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="40"/>
-      <c r="B6" s="33" t="s">
+      <c r="A6" s="65"/>
+      <c r="B6" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="33"/>
+      <c r="C6" s="67"/>
       <c r="D6" s="8"/>
-      <c r="E6" s="46" t="s">
+      <c r="E6" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="44"/>
-      <c r="G6" s="44"/>
-      <c r="H6" s="45"/>
+      <c r="F6" s="53"/>
+      <c r="G6" s="53"/>
+      <c r="H6" s="54"/>
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
       <c r="K6" s="9"/>
@@ -1639,9 +1639,9 @@
       <c r="AE6" s="10"/>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A7" s="40"/>
-      <c r="B7" s="33"/>
-      <c r="C7" s="33"/>
+      <c r="A7" s="65"/>
+      <c r="B7" s="67"/>
+      <c r="C7" s="67"/>
       <c r="D7" s="12"/>
       <c r="E7" s="31"/>
       <c r="F7" s="14"/>
@@ -1672,18 +1672,18 @@
       <c r="AE7" s="14"/>
     </row>
     <row r="8" spans="1:31" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="40" t="s">
+      <c r="A8" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="33" t="s">
+      <c r="B8" s="67" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="33"/>
-      <c r="D8" s="43" t="s">
+      <c r="C8" s="67"/>
+      <c r="D8" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="E8" s="44"/>
-      <c r="F8" s="47"/>
+      <c r="E8" s="53"/>
+      <c r="F8" s="59"/>
       <c r="G8" s="8"/>
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
@@ -1711,9 +1711,9 @@
       <c r="AE8" s="10"/>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A9" s="40"/>
-      <c r="B9" s="33"/>
-      <c r="C9" s="33"/>
+      <c r="A9" s="65"/>
+      <c r="B9" s="67"/>
+      <c r="C9" s="67"/>
       <c r="D9" s="30"/>
       <c r="E9" s="31"/>
       <c r="F9" s="14"/>
@@ -1744,23 +1744,23 @@
       <c r="AE9" s="14"/>
     </row>
     <row r="10" spans="1:31" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="40"/>
-      <c r="B10" s="33" t="s">
+      <c r="A10" s="65"/>
+      <c r="B10" s="67" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="33"/>
-      <c r="D10" s="43" t="s">
+      <c r="C10" s="67"/>
+      <c r="D10" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="E10" s="44"/>
-      <c r="F10" s="47"/>
+      <c r="E10" s="53"/>
+      <c r="F10" s="59"/>
       <c r="G10" s="8"/>
-      <c r="H10" s="46" t="s">
+      <c r="H10" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="I10" s="44"/>
-      <c r="J10" s="44"/>
-      <c r="K10" s="45"/>
+      <c r="I10" s="53"/>
+      <c r="J10" s="53"/>
+      <c r="K10" s="54"/>
       <c r="L10" s="9"/>
       <c r="M10" s="10"/>
       <c r="N10" s="8"/>
@@ -1783,14 +1783,14 @@
       <c r="AE10" s="10"/>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A11" s="40"/>
-      <c r="B11" s="33"/>
-      <c r="C11" s="33"/>
+      <c r="A11" s="65"/>
+      <c r="B11" s="67"/>
+      <c r="C11" s="67"/>
       <c r="D11" s="30"/>
       <c r="E11" s="31"/>
-      <c r="F11" s="62"/>
+      <c r="F11" s="32"/>
       <c r="G11" s="12"/>
-      <c r="H11" s="63"/>
+      <c r="H11" s="33"/>
       <c r="I11" s="13"/>
       <c r="J11" s="13"/>
       <c r="K11" s="13"/>
@@ -1816,26 +1816,26 @@
       <c r="AE11" s="14"/>
     </row>
     <row r="12" spans="1:31" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="32" t="s">
+      <c r="A12" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="38" t="s">
+      <c r="B12" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="34" t="s">
+      <c r="C12" s="64" t="s">
         <v>6</v>
       </c>
       <c r="D12" s="8"/>
       <c r="E12" s="9"/>
       <c r="F12" s="10"/>
       <c r="G12" s="8"/>
-      <c r="H12" s="48" t="s">
+      <c r="H12" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="I12" s="49"/>
-      <c r="J12" s="49"/>
-      <c r="K12" s="49"/>
-      <c r="L12" s="50"/>
+      <c r="I12" s="42"/>
+      <c r="J12" s="42"/>
+      <c r="K12" s="42"/>
+      <c r="L12" s="43"/>
       <c r="M12" s="10"/>
       <c r="N12" s="8"/>
       <c r="O12" s="9"/>
@@ -1845,13 +1845,13 @@
       <c r="S12" s="9"/>
       <c r="T12" s="10"/>
       <c r="U12" s="8"/>
-      <c r="V12" s="51" t="s">
+      <c r="V12" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="W12" s="52"/>
-      <c r="X12" s="52"/>
-      <c r="Y12" s="52"/>
-      <c r="Z12" s="55"/>
+      <c r="W12" s="39"/>
+      <c r="X12" s="39"/>
+      <c r="Y12" s="39"/>
+      <c r="Z12" s="40"/>
       <c r="AA12" s="10"/>
       <c r="AB12" s="11"/>
       <c r="AC12" s="9"/>
@@ -1859,16 +1859,16 @@
       <c r="AE12" s="10"/>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A13" s="32"/>
-      <c r="B13" s="42"/>
-      <c r="C13" s="34"/>
+      <c r="A13" s="66"/>
+      <c r="B13" s="57"/>
+      <c r="C13" s="64"/>
       <c r="D13" s="12"/>
       <c r="E13" s="13"/>
       <c r="F13" s="14"/>
       <c r="G13" s="12"/>
-      <c r="H13" s="66"/>
-      <c r="I13" s="66"/>
-      <c r="J13" s="66"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="36"/>
+      <c r="J13" s="36"/>
       <c r="K13" s="13"/>
       <c r="L13" s="13"/>
       <c r="M13" s="14"/>
@@ -1892,9 +1892,9 @@
       <c r="AE13" s="14"/>
     </row>
     <row r="14" spans="1:31" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="32"/>
-      <c r="B14" s="42"/>
-      <c r="C14" s="34" t="s">
+      <c r="A14" s="66"/>
+      <c r="B14" s="57"/>
+      <c r="C14" s="64" t="s">
         <v>7</v>
       </c>
       <c r="D14" s="8"/>
@@ -1903,46 +1903,46 @@
       <c r="G14" s="8"/>
       <c r="H14" s="9"/>
       <c r="I14" s="9"/>
-      <c r="J14" s="48" t="s">
+      <c r="J14" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="K14" s="49"/>
-      <c r="L14" s="49"/>
-      <c r="M14" s="49"/>
-      <c r="N14" s="49"/>
-      <c r="O14" s="49"/>
-      <c r="P14" s="49"/>
-      <c r="Q14" s="49"/>
-      <c r="R14" s="49"/>
-      <c r="S14" s="50"/>
+      <c r="K14" s="42"/>
+      <c r="L14" s="42"/>
+      <c r="M14" s="42"/>
+      <c r="N14" s="42"/>
+      <c r="O14" s="42"/>
+      <c r="P14" s="42"/>
+      <c r="Q14" s="42"/>
+      <c r="R14" s="42"/>
+      <c r="S14" s="43"/>
       <c r="T14" s="10"/>
       <c r="U14" s="8"/>
       <c r="V14" s="9"/>
-      <c r="W14" s="51" t="s">
+      <c r="W14" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="X14" s="52"/>
-      <c r="Y14" s="52"/>
-      <c r="Z14" s="52"/>
-      <c r="AA14" s="52"/>
-      <c r="AB14" s="52"/>
-      <c r="AC14" s="55"/>
+      <c r="X14" s="39"/>
+      <c r="Y14" s="39"/>
+      <c r="Z14" s="39"/>
+      <c r="AA14" s="39"/>
+      <c r="AB14" s="39"/>
+      <c r="AC14" s="40"/>
       <c r="AD14" s="9"/>
       <c r="AE14" s="10"/>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A15" s="32"/>
-      <c r="B15" s="39"/>
-      <c r="C15" s="34"/>
+      <c r="A15" s="66"/>
+      <c r="B15" s="58"/>
+      <c r="C15" s="64"/>
       <c r="D15" s="12"/>
       <c r="E15" s="13"/>
       <c r="F15" s="14"/>
       <c r="G15" s="12"/>
       <c r="H15" s="13"/>
       <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="13"/>
+      <c r="J15" s="36"/>
+      <c r="K15" s="36"/>
+      <c r="L15" s="36"/>
       <c r="M15" s="14"/>
       <c r="N15" s="12"/>
       <c r="O15" s="13"/>
@@ -1964,11 +1964,11 @@
       <c r="AE15" s="14"/>
     </row>
     <row r="16" spans="1:31" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="32"/>
-      <c r="B16" s="38" t="s">
+      <c r="A16" s="66"/>
+      <c r="B16" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="38" t="s">
+      <c r="C16" s="56" t="s">
         <v>31</v>
       </c>
       <c r="D16" s="8"/>
@@ -1976,13 +1976,13 @@
       <c r="F16" s="10"/>
       <c r="G16" s="8"/>
       <c r="H16" s="9"/>
-      <c r="I16" s="48" t="s">
+      <c r="I16" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="J16" s="49"/>
-      <c r="K16" s="49"/>
-      <c r="L16" s="49"/>
-      <c r="M16" s="54"/>
+      <c r="J16" s="42"/>
+      <c r="K16" s="42"/>
+      <c r="L16" s="42"/>
+      <c r="M16" s="51"/>
       <c r="N16" s="8"/>
       <c r="O16" s="9"/>
       <c r="P16" s="9"/>
@@ -1992,31 +1992,31 @@
       <c r="T16" s="10"/>
       <c r="U16" s="8"/>
       <c r="V16" s="9"/>
-      <c r="W16" s="51" t="s">
+      <c r="W16" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="X16" s="52"/>
-      <c r="Y16" s="52"/>
-      <c r="Z16" s="52"/>
-      <c r="AA16" s="52"/>
-      <c r="AB16" s="52"/>
-      <c r="AC16" s="55"/>
+      <c r="X16" s="39"/>
+      <c r="Y16" s="39"/>
+      <c r="Z16" s="39"/>
+      <c r="AA16" s="39"/>
+      <c r="AB16" s="39"/>
+      <c r="AC16" s="40"/>
       <c r="AD16" s="9"/>
       <c r="AE16" s="10"/>
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A17" s="32"/>
-      <c r="B17" s="42"/>
-      <c r="C17" s="39"/>
+      <c r="A17" s="66"/>
+      <c r="B17" s="57"/>
+      <c r="C17" s="58"/>
       <c r="D17" s="12"/>
       <c r="E17" s="13"/>
       <c r="F17" s="14"/>
       <c r="G17" s="12"/>
-      <c r="H17" s="66"/>
-      <c r="I17" s="66"/>
-      <c r="J17" s="66"/>
-      <c r="K17" s="13"/>
-      <c r="L17" s="13"/>
+      <c r="H17" s="36"/>
+      <c r="I17" s="36"/>
+      <c r="J17" s="36"/>
+      <c r="K17" s="36"/>
+      <c r="L17" s="36"/>
       <c r="M17" s="14"/>
       <c r="N17" s="12"/>
       <c r="O17" s="13"/>
@@ -2038,9 +2038,9 @@
       <c r="AE17" s="14"/>
     </row>
     <row r="18" spans="1:31" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="32"/>
-      <c r="B18" s="42"/>
-      <c r="C18" s="38" t="s">
+      <c r="A18" s="66"/>
+      <c r="B18" s="57"/>
+      <c r="C18" s="56" t="s">
         <v>9</v>
       </c>
       <c r="D18" s="8"/>
@@ -2050,36 +2050,36 @@
       <c r="H18" s="9"/>
       <c r="I18" s="9"/>
       <c r="J18" s="9"/>
-      <c r="K18" s="48" t="s">
+      <c r="K18" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="L18" s="49"/>
-      <c r="M18" s="49"/>
-      <c r="N18" s="49"/>
-      <c r="O18" s="49"/>
-      <c r="P18" s="49"/>
-      <c r="Q18" s="49"/>
-      <c r="R18" s="49"/>
-      <c r="S18" s="50"/>
+      <c r="L18" s="42"/>
+      <c r="M18" s="42"/>
+      <c r="N18" s="42"/>
+      <c r="O18" s="42"/>
+      <c r="P18" s="42"/>
+      <c r="Q18" s="42"/>
+      <c r="R18" s="42"/>
+      <c r="S18" s="43"/>
       <c r="T18" s="10"/>
       <c r="U18" s="8"/>
       <c r="V18" s="9"/>
-      <c r="W18" s="51" t="s">
+      <c r="W18" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="X18" s="52"/>
-      <c r="Y18" s="52"/>
-      <c r="Z18" s="52"/>
-      <c r="AA18" s="52"/>
-      <c r="AB18" s="52"/>
-      <c r="AC18" s="55"/>
+      <c r="X18" s="39"/>
+      <c r="Y18" s="39"/>
+      <c r="Z18" s="39"/>
+      <c r="AA18" s="39"/>
+      <c r="AB18" s="39"/>
+      <c r="AC18" s="40"/>
       <c r="AD18" s="9"/>
       <c r="AE18" s="10"/>
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A19" s="32"/>
-      <c r="B19" s="42"/>
-      <c r="C19" s="39"/>
+      <c r="A19" s="66"/>
+      <c r="B19" s="57"/>
+      <c r="C19" s="58"/>
       <c r="D19" s="12"/>
       <c r="E19" s="13"/>
       <c r="F19" s="14"/>
@@ -2110,9 +2110,9 @@
       <c r="AE19" s="14"/>
     </row>
     <row r="20" spans="1:31" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="32"/>
-      <c r="B20" s="42"/>
-      <c r="C20" s="38" t="s">
+      <c r="A20" s="66"/>
+      <c r="B20" s="57"/>
+      <c r="C20" s="56" t="s">
         <v>10</v>
       </c>
       <c r="D20" s="8"/>
@@ -2122,36 +2122,36 @@
       <c r="H20" s="9"/>
       <c r="I20" s="9"/>
       <c r="J20" s="9"/>
-      <c r="K20" s="48" t="s">
+      <c r="K20" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="L20" s="49"/>
-      <c r="M20" s="49"/>
-      <c r="N20" s="49"/>
-      <c r="O20" s="49"/>
-      <c r="P20" s="49"/>
-      <c r="Q20" s="49"/>
-      <c r="R20" s="49"/>
-      <c r="S20" s="50"/>
+      <c r="L20" s="42"/>
+      <c r="M20" s="42"/>
+      <c r="N20" s="42"/>
+      <c r="O20" s="42"/>
+      <c r="P20" s="42"/>
+      <c r="Q20" s="42"/>
+      <c r="R20" s="42"/>
+      <c r="S20" s="43"/>
       <c r="T20" s="10"/>
       <c r="U20" s="8"/>
       <c r="V20" s="9"/>
-      <c r="W20" s="51" t="s">
+      <c r="W20" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="X20" s="52"/>
-      <c r="Y20" s="52"/>
-      <c r="Z20" s="52"/>
-      <c r="AA20" s="52"/>
-      <c r="AB20" s="52"/>
-      <c r="AC20" s="55"/>
+      <c r="X20" s="39"/>
+      <c r="Y20" s="39"/>
+      <c r="Z20" s="39"/>
+      <c r="AA20" s="39"/>
+      <c r="AB20" s="39"/>
+      <c r="AC20" s="40"/>
       <c r="AD20" s="9"/>
       <c r="AE20" s="10"/>
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A21" s="32"/>
-      <c r="B21" s="42"/>
-      <c r="C21" s="39"/>
+      <c r="A21" s="66"/>
+      <c r="B21" s="57"/>
+      <c r="C21" s="58"/>
       <c r="D21" s="12"/>
       <c r="E21" s="13"/>
       <c r="F21" s="14"/>
@@ -2182,11 +2182,11 @@
       <c r="AE21" s="14"/>
     </row>
     <row r="22" spans="1:31" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="32"/>
-      <c r="B22" s="38" t="s">
+      <c r="A22" s="66"/>
+      <c r="B22" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="34" t="s">
+      <c r="C22" s="64" t="s">
         <v>11</v>
       </c>
       <c r="D22" s="25"/>
@@ -2195,18 +2195,18 @@
       <c r="G22" s="25"/>
       <c r="H22" s="26"/>
       <c r="I22" s="26"/>
-      <c r="J22" s="59" t="s">
+      <c r="J22" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="K22" s="60"/>
-      <c r="L22" s="60"/>
-      <c r="M22" s="60"/>
-      <c r="N22" s="60"/>
-      <c r="O22" s="60"/>
-      <c r="P22" s="60"/>
-      <c r="Q22" s="60"/>
-      <c r="R22" s="60"/>
-      <c r="S22" s="61"/>
+      <c r="K22" s="48"/>
+      <c r="L22" s="48"/>
+      <c r="M22" s="48"/>
+      <c r="N22" s="48"/>
+      <c r="O22" s="48"/>
+      <c r="P22" s="48"/>
+      <c r="Q22" s="48"/>
+      <c r="R22" s="48"/>
+      <c r="S22" s="49"/>
       <c r="T22" s="27"/>
       <c r="U22" s="25"/>
       <c r="V22" s="26"/>
@@ -2221,18 +2221,18 @@
       <c r="AE22" s="27"/>
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A23" s="32"/>
-      <c r="B23" s="42"/>
-      <c r="C23" s="34"/>
+      <c r="A23" s="66"/>
+      <c r="B23" s="57"/>
+      <c r="C23" s="64"/>
       <c r="D23" s="23"/>
       <c r="E23" s="21"/>
       <c r="F23" s="22"/>
       <c r="G23" s="23"/>
-      <c r="H23" s="67"/>
-      <c r="I23" s="67"/>
-      <c r="J23" s="67"/>
-      <c r="K23" s="21"/>
-      <c r="L23" s="21"/>
+      <c r="H23" s="37"/>
+      <c r="I23" s="37"/>
+      <c r="J23" s="37"/>
+      <c r="K23" s="37"/>
+      <c r="L23" s="37"/>
       <c r="M23" s="22"/>
       <c r="N23" s="23"/>
       <c r="O23" s="21"/>
@@ -2254,9 +2254,9 @@
       <c r="AE23" s="22"/>
     </row>
     <row r="24" spans="1:31" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="32"/>
-      <c r="B24" s="42"/>
-      <c r="C24" s="34" t="s">
+      <c r="A24" s="66"/>
+      <c r="B24" s="57"/>
+      <c r="C24" s="64" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="17"/>
@@ -2272,32 +2272,32 @@
       <c r="N24" s="17"/>
       <c r="O24" s="18"/>
       <c r="P24" s="18"/>
-      <c r="Q24" s="59" t="s">
+      <c r="Q24" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="R24" s="60"/>
-      <c r="S24" s="60"/>
-      <c r="T24" s="60"/>
-      <c r="U24" s="60"/>
-      <c r="V24" s="60"/>
-      <c r="W24" s="60"/>
-      <c r="X24" s="61"/>
+      <c r="R24" s="48"/>
+      <c r="S24" s="48"/>
+      <c r="T24" s="48"/>
+      <c r="U24" s="48"/>
+      <c r="V24" s="48"/>
+      <c r="W24" s="48"/>
+      <c r="X24" s="49"/>
       <c r="Y24" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="Z24" s="56" t="s">
+      <c r="Z24" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="AA24" s="57"/>
-      <c r="AB24" s="57"/>
-      <c r="AC24" s="58"/>
+      <c r="AA24" s="45"/>
+      <c r="AB24" s="45"/>
+      <c r="AC24" s="46"/>
       <c r="AD24" s="18"/>
       <c r="AE24" s="19"/>
     </row>
     <row r="25" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A25" s="32"/>
-      <c r="B25" s="39"/>
-      <c r="C25" s="34"/>
+      <c r="A25" s="66"/>
+      <c r="B25" s="58"/>
+      <c r="C25" s="64"/>
       <c r="D25" s="17"/>
       <c r="E25" s="18"/>
       <c r="F25" s="19"/>
@@ -2328,11 +2328,11 @@
       <c r="AE25" s="19"/>
     </row>
     <row r="26" spans="1:31" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="32"/>
-      <c r="B26" s="34" t="s">
+      <c r="A26" s="66"/>
+      <c r="B26" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="C26" s="34" t="s">
+      <c r="C26" s="64" t="s">
         <v>17</v>
       </c>
       <c r="D26" s="8"/>
@@ -2346,32 +2346,32 @@
       <c r="L26" s="9"/>
       <c r="M26" s="10"/>
       <c r="N26" s="8"/>
-      <c r="O26" s="48" t="s">
+      <c r="O26" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="P26" s="49"/>
-      <c r="Q26" s="49"/>
-      <c r="R26" s="49"/>
-      <c r="S26" s="50"/>
+      <c r="P26" s="42"/>
+      <c r="Q26" s="42"/>
+      <c r="R26" s="42"/>
+      <c r="S26" s="43"/>
       <c r="T26" s="10"/>
       <c r="U26" s="8"/>
-      <c r="V26" s="51" t="s">
+      <c r="V26" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="W26" s="52"/>
-      <c r="X26" s="52"/>
-      <c r="Y26" s="52"/>
-      <c r="Z26" s="52"/>
-      <c r="AA26" s="52"/>
-      <c r="AB26" s="52"/>
-      <c r="AC26" s="55"/>
+      <c r="W26" s="39"/>
+      <c r="X26" s="39"/>
+      <c r="Y26" s="39"/>
+      <c r="Z26" s="39"/>
+      <c r="AA26" s="39"/>
+      <c r="AB26" s="39"/>
+      <c r="AC26" s="40"/>
       <c r="AD26" s="9"/>
       <c r="AE26" s="10"/>
     </row>
     <row r="27" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A27" s="32"/>
-      <c r="B27" s="34"/>
-      <c r="C27" s="34"/>
+      <c r="A27" s="66"/>
+      <c r="B27" s="64"/>
+      <c r="C27" s="64"/>
       <c r="D27" s="12"/>
       <c r="E27" s="13"/>
       <c r="F27" s="14"/>
@@ -2402,9 +2402,9 @@
       <c r="AE27" s="14"/>
     </row>
     <row r="28" spans="1:31" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="32"/>
-      <c r="B28" s="34"/>
-      <c r="C28" s="34" t="s">
+      <c r="A28" s="66"/>
+      <c r="B28" s="64"/>
+      <c r="C28" s="64" t="s">
         <v>16</v>
       </c>
       <c r="D28" s="8"/>
@@ -2414,44 +2414,44 @@
       <c r="H28" s="9"/>
       <c r="I28" s="9"/>
       <c r="J28" s="9"/>
-      <c r="K28" s="48" t="s">
+      <c r="K28" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="L28" s="49"/>
-      <c r="M28" s="49"/>
-      <c r="N28" s="49"/>
-      <c r="O28" s="49"/>
-      <c r="P28" s="49"/>
-      <c r="Q28" s="49"/>
-      <c r="R28" s="49"/>
-      <c r="S28" s="50"/>
+      <c r="L28" s="42"/>
+      <c r="M28" s="42"/>
+      <c r="N28" s="42"/>
+      <c r="O28" s="42"/>
+      <c r="P28" s="42"/>
+      <c r="Q28" s="42"/>
+      <c r="R28" s="42"/>
+      <c r="S28" s="43"/>
       <c r="T28" s="10"/>
       <c r="U28" s="8"/>
-      <c r="V28" s="51" t="s">
+      <c r="V28" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="W28" s="52"/>
-      <c r="X28" s="52"/>
-      <c r="Y28" s="52"/>
-      <c r="Z28" s="52"/>
-      <c r="AA28" s="52"/>
-      <c r="AB28" s="52"/>
-      <c r="AC28" s="55"/>
+      <c r="W28" s="39"/>
+      <c r="X28" s="39"/>
+      <c r="Y28" s="39"/>
+      <c r="Z28" s="39"/>
+      <c r="AA28" s="39"/>
+      <c r="AB28" s="39"/>
+      <c r="AC28" s="40"/>
       <c r="AD28" s="9"/>
       <c r="AE28" s="10"/>
     </row>
     <row r="29" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A29" s="32"/>
-      <c r="B29" s="34"/>
-      <c r="C29" s="34"/>
+      <c r="A29" s="66"/>
+      <c r="B29" s="64"/>
+      <c r="C29" s="64"/>
       <c r="D29" s="12"/>
       <c r="E29" s="13"/>
       <c r="F29" s="14"/>
       <c r="G29" s="12"/>
       <c r="H29" s="13"/>
-      <c r="I29" s="66"/>
-      <c r="J29" s="66"/>
-      <c r="K29" s="13"/>
+      <c r="I29" s="36"/>
+      <c r="J29" s="36"/>
+      <c r="K29" s="36"/>
       <c r="L29" s="13"/>
       <c r="M29" s="14"/>
       <c r="N29" s="12"/>
@@ -2474,9 +2474,9 @@
       <c r="AE29" s="14"/>
     </row>
     <row r="30" spans="1:31" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="32"/>
-      <c r="B30" s="34"/>
-      <c r="C30" s="34" t="s">
+      <c r="A30" s="66"/>
+      <c r="B30" s="64"/>
+      <c r="C30" s="64" t="s">
         <v>13</v>
       </c>
       <c r="D30" s="8"/>
@@ -2486,36 +2486,36 @@
       <c r="H30" s="9"/>
       <c r="I30" s="9"/>
       <c r="J30" s="9"/>
-      <c r="K30" s="48" t="s">
+      <c r="K30" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="L30" s="49"/>
-      <c r="M30" s="49"/>
-      <c r="N30" s="49"/>
-      <c r="O30" s="49"/>
-      <c r="P30" s="49"/>
-      <c r="Q30" s="49"/>
-      <c r="R30" s="49"/>
-      <c r="S30" s="50"/>
+      <c r="L30" s="42"/>
+      <c r="M30" s="42"/>
+      <c r="N30" s="42"/>
+      <c r="O30" s="42"/>
+      <c r="P30" s="42"/>
+      <c r="Q30" s="42"/>
+      <c r="R30" s="42"/>
+      <c r="S30" s="43"/>
       <c r="T30" s="10"/>
       <c r="U30" s="8"/>
-      <c r="V30" s="51" t="s">
+      <c r="V30" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="W30" s="52"/>
-      <c r="X30" s="52"/>
-      <c r="Y30" s="52"/>
-      <c r="Z30" s="52"/>
-      <c r="AA30" s="52"/>
-      <c r="AB30" s="52"/>
-      <c r="AC30" s="55"/>
+      <c r="W30" s="39"/>
+      <c r="X30" s="39"/>
+      <c r="Y30" s="39"/>
+      <c r="Z30" s="39"/>
+      <c r="AA30" s="39"/>
+      <c r="AB30" s="39"/>
+      <c r="AC30" s="40"/>
       <c r="AD30" s="9"/>
       <c r="AE30" s="10"/>
     </row>
     <row r="31" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A31" s="32"/>
-      <c r="B31" s="34"/>
-      <c r="C31" s="34"/>
+      <c r="A31" s="66"/>
+      <c r="B31" s="64"/>
+      <c r="C31" s="64"/>
       <c r="D31" s="12"/>
       <c r="E31" s="13"/>
       <c r="F31" s="14"/>
@@ -2523,8 +2523,8 @@
       <c r="H31" s="13"/>
       <c r="I31" s="13"/>
       <c r="J31" s="13"/>
-      <c r="K31" s="13"/>
-      <c r="L31" s="13"/>
+      <c r="K31" s="36"/>
+      <c r="L31" s="36"/>
       <c r="M31" s="14"/>
       <c r="N31" s="12"/>
       <c r="O31" s="13"/>
@@ -2546,22 +2546,22 @@
       <c r="AE31" s="14"/>
     </row>
     <row r="32" spans="1:31" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="32"/>
-      <c r="B32" s="34"/>
-      <c r="C32" s="34" t="s">
+      <c r="A32" s="66"/>
+      <c r="B32" s="64"/>
+      <c r="C32" s="64" t="s">
         <v>14</v>
       </c>
       <c r="D32" s="8"/>
       <c r="E32" s="9"/>
       <c r="F32" s="10"/>
       <c r="G32" s="8"/>
-      <c r="H32" s="48" t="s">
+      <c r="H32" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="I32" s="49"/>
-      <c r="J32" s="49"/>
-      <c r="K32" s="49"/>
-      <c r="L32" s="50"/>
+      <c r="I32" s="42"/>
+      <c r="J32" s="42"/>
+      <c r="K32" s="42"/>
+      <c r="L32" s="43"/>
       <c r="M32" s="10"/>
       <c r="N32" s="8"/>
       <c r="O32" s="9"/>
@@ -2571,29 +2571,29 @@
       <c r="S32" s="9"/>
       <c r="T32" s="10"/>
       <c r="U32" s="8"/>
-      <c r="V32" s="51" t="s">
+      <c r="V32" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="W32" s="52"/>
-      <c r="X32" s="52"/>
-      <c r="Y32" s="52"/>
-      <c r="Z32" s="52"/>
-      <c r="AA32" s="52"/>
-      <c r="AB32" s="52"/>
-      <c r="AC32" s="55"/>
+      <c r="W32" s="39"/>
+      <c r="X32" s="39"/>
+      <c r="Y32" s="39"/>
+      <c r="Z32" s="39"/>
+      <c r="AA32" s="39"/>
+      <c r="AB32" s="39"/>
+      <c r="AC32" s="40"/>
       <c r="AD32" s="9"/>
       <c r="AE32" s="10"/>
     </row>
     <row r="33" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A33" s="32"/>
-      <c r="B33" s="34"/>
-      <c r="C33" s="34"/>
+      <c r="A33" s="66"/>
+      <c r="B33" s="64"/>
+      <c r="C33" s="64"/>
       <c r="D33" s="12"/>
       <c r="E33" s="13"/>
-      <c r="F33" s="64"/>
-      <c r="G33" s="65"/>
-      <c r="H33" s="66"/>
-      <c r="I33" s="66"/>
+      <c r="F33" s="34"/>
+      <c r="G33" s="35"/>
+      <c r="H33" s="36"/>
+      <c r="I33" s="36"/>
       <c r="J33" s="13"/>
       <c r="K33" s="13"/>
       <c r="L33" s="13"/>
@@ -2618,22 +2618,22 @@
       <c r="AE33" s="14"/>
     </row>
     <row r="34" spans="1:31" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="32"/>
-      <c r="B34" s="34"/>
-      <c r="C34" s="34" t="s">
+      <c r="A34" s="66"/>
+      <c r="B34" s="64"/>
+      <c r="C34" s="64" t="s">
         <v>15</v>
       </c>
       <c r="D34" s="8"/>
       <c r="E34" s="9"/>
       <c r="F34" s="10"/>
       <c r="G34" s="8"/>
-      <c r="H34" s="48" t="s">
+      <c r="H34" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="I34" s="49"/>
-      <c r="J34" s="49"/>
-      <c r="K34" s="49"/>
-      <c r="L34" s="50"/>
+      <c r="I34" s="42"/>
+      <c r="J34" s="42"/>
+      <c r="K34" s="42"/>
+      <c r="L34" s="43"/>
       <c r="M34" s="10"/>
       <c r="N34" s="8"/>
       <c r="O34" s="9"/>
@@ -2643,13 +2643,13 @@
       <c r="S34" s="9"/>
       <c r="T34" s="10"/>
       <c r="U34" s="8"/>
-      <c r="V34" s="51" t="s">
+      <c r="V34" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="W34" s="52"/>
-      <c r="X34" s="52"/>
-      <c r="Y34" s="52"/>
-      <c r="Z34" s="55"/>
+      <c r="W34" s="39"/>
+      <c r="X34" s="39"/>
+      <c r="Y34" s="39"/>
+      <c r="Z34" s="40"/>
       <c r="AA34" s="10"/>
       <c r="AB34" s="11"/>
       <c r="AC34" s="9"/>
@@ -2657,15 +2657,15 @@
       <c r="AE34" s="10"/>
     </row>
     <row r="35" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A35" s="32"/>
-      <c r="B35" s="34"/>
-      <c r="C35" s="34"/>
+      <c r="A35" s="66"/>
+      <c r="B35" s="64"/>
+      <c r="C35" s="64"/>
       <c r="D35" s="12"/>
       <c r="E35" s="13"/>
-      <c r="F35" s="64"/>
-      <c r="G35" s="65"/>
-      <c r="H35" s="66"/>
-      <c r="I35" s="66"/>
+      <c r="F35" s="34"/>
+      <c r="G35" s="35"/>
+      <c r="H35" s="36"/>
+      <c r="I35" s="36"/>
       <c r="J35" s="13"/>
       <c r="K35" s="13"/>
       <c r="L35" s="13"/>
@@ -2690,13 +2690,13 @@
       <c r="AE35" s="14"/>
     </row>
     <row r="36" spans="1:31" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="36" t="s">
+      <c r="A36" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="B36" s="35" t="s">
+      <c r="B36" s="62" t="s">
         <v>28</v>
       </c>
-      <c r="C36" s="35"/>
+      <c r="C36" s="62"/>
       <c r="D36" s="8"/>
       <c r="E36" s="9"/>
       <c r="F36" s="10"/>
@@ -2722,16 +2722,16 @@
       <c r="Z36" s="9"/>
       <c r="AA36" s="10"/>
       <c r="AB36" s="11"/>
-      <c r="AC36" s="51" t="s">
+      <c r="AC36" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="AD36" s="52"/>
-      <c r="AE36" s="53"/>
+      <c r="AD36" s="39"/>
+      <c r="AE36" s="50"/>
     </row>
     <row r="37" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A37" s="36"/>
-      <c r="B37" s="35"/>
-      <c r="C37" s="35"/>
+      <c r="A37" s="63"/>
+      <c r="B37" s="62"/>
+      <c r="C37" s="62"/>
       <c r="D37" s="12"/>
       <c r="E37" s="13"/>
       <c r="F37" s="14"/>
@@ -2795,6 +2795,52 @@
     </row>
   </sheetData>
   <mergeCells count="62">
+    <mergeCell ref="A12:A35"/>
+    <mergeCell ref="B10:C11"/>
+    <mergeCell ref="B8:C9"/>
+    <mergeCell ref="B6:C7"/>
+    <mergeCell ref="B4:C5"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="B16:B21"/>
+    <mergeCell ref="B36:C37"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:M2"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="B26:B35"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="U2:AA2"/>
+    <mergeCell ref="AB2:AE2"/>
+    <mergeCell ref="D1:AA1"/>
+    <mergeCell ref="AB1:AE1"/>
+    <mergeCell ref="A1:C3"/>
+    <mergeCell ref="N2:T2"/>
+    <mergeCell ref="D4:H4"/>
+    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="H12:L12"/>
+    <mergeCell ref="AC36:AE36"/>
+    <mergeCell ref="J14:S14"/>
+    <mergeCell ref="I16:M16"/>
+    <mergeCell ref="K18:S18"/>
+    <mergeCell ref="K20:S20"/>
+    <mergeCell ref="H32:L32"/>
+    <mergeCell ref="J22:S22"/>
     <mergeCell ref="V12:Z12"/>
     <mergeCell ref="V32:AC32"/>
     <mergeCell ref="V30:AC30"/>
@@ -2811,52 +2857,6 @@
     <mergeCell ref="W18:AC18"/>
     <mergeCell ref="W20:AC20"/>
     <mergeCell ref="Q24:X24"/>
-    <mergeCell ref="AC36:AE36"/>
-    <mergeCell ref="J14:S14"/>
-    <mergeCell ref="I16:M16"/>
-    <mergeCell ref="K18:S18"/>
-    <mergeCell ref="K20:S20"/>
-    <mergeCell ref="H32:L32"/>
-    <mergeCell ref="J22:S22"/>
-    <mergeCell ref="D4:H4"/>
-    <mergeCell ref="E6:H6"/>
-    <mergeCell ref="B12:B15"/>
-    <mergeCell ref="H10:K10"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="H12:L12"/>
-    <mergeCell ref="U2:AA2"/>
-    <mergeCell ref="AB2:AE2"/>
-    <mergeCell ref="D1:AA1"/>
-    <mergeCell ref="AB1:AE1"/>
-    <mergeCell ref="A1:C3"/>
-    <mergeCell ref="N2:T2"/>
-    <mergeCell ref="B36:C37"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="G2:M2"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="B26:B35"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="A12:A35"/>
-    <mergeCell ref="B10:C11"/>
-    <mergeCell ref="B8:C9"/>
-    <mergeCell ref="B6:C7"/>
-    <mergeCell ref="B4:C5"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="B16:B21"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>